<commit_message>
COnvert results to 3dp
</commit_message>
<xml_diff>
--- a/sentiment_results.xlsx
+++ b/sentiment_results.xlsx
@@ -2889,25 +2889,23 @@
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="n">
-        <v>0.9559683799743652</v>
+        <v>0.956</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1952711045742035</v>
+        <v>0.195</v>
       </c>
       <c r="S3" t="n">
-        <v>0.1866730014956062</v>
+        <v>0.187</v>
       </c>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
-      <c r="W3" t="n">
-        <v>8.842998795444146e-05</v>
-      </c>
+      <c r="W3" t="inlineStr"/>
       <c r="X3" t="n">
-        <v>0.289983719587326</v>
+        <v>0.29</v>
       </c>
       <c r="Y3" t="n">
-        <v>2.564325683009137e-05</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
@@ -2939,14 +2937,12 @@
       <c r="BA3" t="inlineStr"/>
       <c r="BB3" t="inlineStr"/>
       <c r="BC3" t="inlineStr"/>
-      <c r="BD3" t="n">
-        <v>8.588640775997192e-05</v>
-      </c>
+      <c r="BD3" t="inlineStr"/>
       <c r="BE3" t="n">
-        <v>0.1689730584621429</v>
+        <v>0.169</v>
       </c>
       <c r="BF3" t="n">
-        <v>1.451248899952918e-05</v>
+        <v>0</v>
       </c>
       <c r="BG3" t="inlineStr"/>
       <c r="BH3" t="inlineStr"/>
@@ -2987,14 +2983,12 @@
       <c r="CQ3" t="inlineStr"/>
       <c r="CR3" t="inlineStr"/>
       <c r="CS3" t="inlineStr"/>
-      <c r="CT3" t="n">
-        <v>8.307590178446844e-05</v>
-      </c>
+      <c r="CT3" t="inlineStr"/>
       <c r="CU3" t="n">
-        <v>0.2672236859798431</v>
+        <v>0.267</v>
       </c>
       <c r="CV3" t="n">
-        <v>2.219984869094509e-05</v>
+        <v>0</v>
       </c>
       <c r="CW3" t="inlineStr"/>
       <c r="CX3" t="inlineStr"/>
@@ -3008,14 +3002,12 @@
       <c r="DF3" t="inlineStr"/>
       <c r="DG3" t="inlineStr"/>
       <c r="DH3" t="inlineStr"/>
-      <c r="DI3" t="n">
-        <v>0.0001174385834019631</v>
-      </c>
+      <c r="DI3" t="inlineStr"/>
       <c r="DJ3" t="n">
-        <v>0.1275320202112198</v>
+        <v>0.128</v>
       </c>
       <c r="DK3" t="n">
-        <v>1.497717979199618e-05</v>
+        <v>0</v>
       </c>
       <c r="DL3" t="inlineStr"/>
       <c r="DM3" t="inlineStr"/>
@@ -3038,14 +3030,12 @@
       <c r="ED3" t="inlineStr"/>
       <c r="EE3" t="inlineStr"/>
       <c r="EF3" t="inlineStr"/>
-      <c r="EG3" t="n">
-        <v>8.604593313066289e-05</v>
-      </c>
+      <c r="EG3" t="inlineStr"/>
       <c r="EH3" t="n">
-        <v>0.2088744938373566</v>
+        <v>0.209</v>
       </c>
       <c r="EI3" t="n">
-        <v>1.797280072943024e-05</v>
+        <v>0</v>
       </c>
       <c r="EJ3" t="inlineStr"/>
       <c r="EK3" t="inlineStr"/>
@@ -3059,26 +3049,22 @@
       <c r="ES3" t="inlineStr"/>
       <c r="ET3" t="inlineStr"/>
       <c r="EU3" t="inlineStr"/>
-      <c r="EV3" t="n">
-        <v>9.834367665462196e-05</v>
-      </c>
+      <c r="EV3" t="inlineStr"/>
       <c r="EW3" t="n">
-        <v>0.2268495559692383</v>
+        <v>0.227</v>
       </c>
       <c r="EX3" t="n">
-        <v>2.230921938148334e-05</v>
+        <v>0</v>
       </c>
       <c r="EY3" t="inlineStr"/>
       <c r="EZ3" t="inlineStr"/>
       <c r="FA3" t="inlineStr"/>
-      <c r="FB3" t="n">
-        <v>8.686914225108922e-05</v>
-      </c>
+      <c r="FB3" t="inlineStr"/>
       <c r="FC3" t="n">
-        <v>0.1161210164427757</v>
+        <v>0.116</v>
       </c>
       <c r="FD3" t="n">
-        <v>1.008733309570855e-05</v>
+        <v>0</v>
       </c>
       <c r="FE3" t="inlineStr"/>
       <c r="FF3" t="inlineStr"/>
@@ -3101,14 +3087,12 @@
       <c r="FW3" t="inlineStr"/>
       <c r="FX3" t="inlineStr"/>
       <c r="FY3" t="inlineStr"/>
-      <c r="FZ3" t="n">
-        <v>8.69993818923831e-05</v>
-      </c>
+      <c r="FZ3" t="inlineStr"/>
       <c r="GA3" t="n">
-        <v>0.1214896067976952</v>
+        <v>0.121</v>
       </c>
       <c r="GB3" t="n">
-        <v>1.056952069774814e-05</v>
+        <v>0</v>
       </c>
       <c r="GC3" t="inlineStr"/>
       <c r="GD3" t="inlineStr"/>
@@ -3155,23 +3139,19 @@
       <c r="HS3" t="inlineStr"/>
       <c r="HT3" t="inlineStr"/>
       <c r="HU3" t="inlineStr"/>
-      <c r="HV3" t="n">
-        <v>9.993308049160987e-05</v>
-      </c>
+      <c r="HV3" t="inlineStr"/>
       <c r="HW3" t="n">
-        <v>0.1087682247161865</v>
+        <v>0.109</v>
       </c>
       <c r="HX3" t="n">
-        <v>1.086954375549218e-05</v>
-      </c>
-      <c r="HY3" t="n">
-        <v>0.0001482830411987379</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="HY3" t="inlineStr"/>
       <c r="HZ3" t="n">
-        <v>0.1235938668251038</v>
+        <v>0.124</v>
       </c>
       <c r="IA3" t="n">
-        <v>1.832687444633819e-05</v>
+        <v>0</v>
       </c>
       <c r="IB3" t="inlineStr"/>
       <c r="IC3" t="inlineStr"/>
@@ -3188,35 +3168,29 @@
       <c r="IN3" t="inlineStr"/>
       <c r="IO3" t="inlineStr"/>
       <c r="IP3" t="inlineStr"/>
-      <c r="IQ3" t="n">
-        <v>9.368468454340473e-05</v>
-      </c>
+      <c r="IQ3" t="inlineStr"/>
       <c r="IR3" t="n">
-        <v>0.151075154542923</v>
+        <v>0.151</v>
       </c>
       <c r="IS3" t="n">
-        <v>1.415342819569986e-05</v>
-      </c>
-      <c r="IT3" t="n">
-        <v>8.566564065404236e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="IT3" t="inlineStr"/>
       <c r="IU3" t="n">
-        <v>0.1354141235351562</v>
+        <v>0.135</v>
       </c>
       <c r="IV3" t="n">
-        <v>1.16003376462448e-05</v>
+        <v>0</v>
       </c>
       <c r="IW3" t="inlineStr"/>
       <c r="IX3" t="inlineStr"/>
       <c r="IY3" t="inlineStr"/>
-      <c r="IZ3" t="n">
-        <v>8.521036943420768e-05</v>
-      </c>
+      <c r="IZ3" t="inlineStr"/>
       <c r="JA3" t="n">
-        <v>0.1389642208814621</v>
+        <v>0.139</v>
       </c>
       <c r="JB3" t="n">
-        <v>1.184119259944622e-05</v>
+        <v>0</v>
       </c>
       <c r="JC3" t="inlineStr"/>
       <c r="JD3" t="inlineStr"/>
@@ -3245,14 +3219,12 @@
       <c r="KA3" t="inlineStr"/>
       <c r="KB3" t="inlineStr"/>
       <c r="KC3" t="inlineStr"/>
-      <c r="KD3" t="n">
-        <v>9.620107448427007e-05</v>
-      </c>
+      <c r="KD3" t="inlineStr"/>
       <c r="KE3" t="n">
-        <v>0.1288064420223236</v>
+        <v>0.129</v>
       </c>
       <c r="KF3" t="n">
-        <v>1.239131812304337e-05</v>
+        <v>0</v>
       </c>
       <c r="KG3" t="inlineStr"/>
       <c r="KH3" t="inlineStr"/>
@@ -3278,14 +3250,12 @@
       <c r="LB3" t="inlineStr"/>
       <c r="LC3" t="inlineStr"/>
       <c r="LD3" t="inlineStr"/>
-      <c r="LE3" t="n">
-        <v>9.089872764889151e-05</v>
-      </c>
+      <c r="LE3" t="inlineStr"/>
       <c r="LF3" t="n">
-        <v>0.1200953498482704</v>
+        <v>0.12</v>
       </c>
       <c r="LG3" t="n">
-        <v>1.091651449775628e-05</v>
+        <v>0</v>
       </c>
       <c r="LH3" t="inlineStr"/>
       <c r="LI3" t="inlineStr"/>
@@ -3296,14 +3266,12 @@
       <c r="LN3" t="inlineStr"/>
       <c r="LO3" t="inlineStr"/>
       <c r="LP3" t="inlineStr"/>
-      <c r="LQ3" t="n">
-        <v>0.0001019966366584413</v>
-      </c>
+      <c r="LQ3" t="inlineStr"/>
       <c r="LR3" t="n">
-        <v>0.1443668305873871</v>
+        <v>0.144</v>
       </c>
       <c r="LS3" t="n">
-        <v>1.472493116495247e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -3313,25 +3281,23 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01220167148858309</v>
+        <v>0.012</v>
       </c>
       <c r="C4" t="n">
-        <v>0.484452486038208</v>
+        <v>0.484</v>
       </c>
       <c r="D4" t="n">
-        <v>0.005911130086465599</v>
+        <v>0.006</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>0.0003726421273313463</v>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>0.3992241024971008</v>
+        <v>0.399</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0001487677188364671</v>
+        <v>0</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -3348,23 +3314,21 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="n">
-        <v>0.0003856650437228382</v>
-      </c>
+      <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="n">
-        <v>0.4888180196285248</v>
+        <v>0.489</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.0001885200229125462</v>
+        <v>0</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.0005201695603318512</v>
+        <v>0.001</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.5235341191291809</v>
+        <v>0.524</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.0002723265125661491</v>
+        <v>0</v>
       </c>
       <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="inlineStr"/>
@@ -3373,13 +3337,13 @@
       <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>
       <c r="AL4" t="n">
-        <v>0.6008694767951965</v>
+        <v>0.601</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.7179864048957825</v>
+        <v>0.718</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.4314161154557929</v>
+        <v>0.431</v>
       </c>
       <c r="AO4" t="inlineStr"/>
       <c r="AP4" t="inlineStr"/>
@@ -3427,22 +3391,20 @@
       <c r="CF4" t="inlineStr"/>
       <c r="CG4" t="inlineStr"/>
       <c r="CH4" t="n">
-        <v>0.9899423122406006</v>
+        <v>0.99</v>
       </c>
       <c r="CI4" t="n">
-        <v>0.4362135827541351</v>
+        <v>0.436</v>
       </c>
       <c r="CJ4" t="n">
-        <v>0.4318262827423851</v>
-      </c>
-      <c r="CK4" t="n">
-        <v>0.0001597608934389427</v>
-      </c>
+        <v>0.432</v>
+      </c>
+      <c r="CK4" t="inlineStr"/>
       <c r="CL4" t="n">
-        <v>0.6286523938179016</v>
+        <v>0.629</v>
       </c>
       <c r="CM4" t="n">
-        <v>0.000100434068098878</v>
+        <v>0</v>
       </c>
       <c r="CN4" t="inlineStr"/>
       <c r="CO4" t="inlineStr"/>
@@ -3456,32 +3418,28 @@
       <c r="CW4" t="inlineStr"/>
       <c r="CX4" t="inlineStr"/>
       <c r="CY4" t="inlineStr"/>
-      <c r="CZ4" t="n">
-        <v>0.0001513736933702603</v>
-      </c>
+      <c r="CZ4" t="inlineStr"/>
       <c r="DA4" t="n">
-        <v>0.6028144955635071</v>
+        <v>0.603</v>
       </c>
       <c r="DB4" t="n">
-        <v>9.125025661057846e-05</v>
+        <v>0</v>
       </c>
       <c r="DC4" t="n">
-        <v>0.9932031631469727</v>
+        <v>0.993</v>
       </c>
       <c r="DD4" t="n">
-        <v>0.4134974479675293</v>
+        <v>0.413</v>
       </c>
       <c r="DE4" t="n">
-        <v>0.4106869732745508</v>
-      </c>
-      <c r="DF4" t="n">
-        <v>0.0001681777357589453</v>
-      </c>
+        <v>0.411</v>
+      </c>
+      <c r="DF4" t="inlineStr"/>
       <c r="DG4" t="n">
-        <v>0.4482145011425018</v>
+        <v>0.448</v>
       </c>
       <c r="DH4" t="n">
-        <v>7.537969993647118e-05</v>
+        <v>0</v>
       </c>
       <c r="DI4" t="inlineStr"/>
       <c r="DJ4" t="inlineStr"/>
@@ -3489,14 +3447,12 @@
       <c r="DL4" t="inlineStr"/>
       <c r="DM4" t="inlineStr"/>
       <c r="DN4" t="inlineStr"/>
-      <c r="DO4" t="n">
-        <v>0.0003448428178671747</v>
-      </c>
+      <c r="DO4" t="inlineStr"/>
       <c r="DP4" t="n">
-        <v>0.3725727498531342</v>
+        <v>0.373</v>
       </c>
       <c r="DQ4" t="n">
-        <v>0.0001284790369198768</v>
+        <v>0</v>
       </c>
       <c r="DR4" t="inlineStr"/>
       <c r="DS4" t="inlineStr"/>
@@ -3520,13 +3476,13 @@
       <c r="EK4" t="inlineStr"/>
       <c r="EL4" t="inlineStr"/>
       <c r="EM4" t="n">
-        <v>0.2613846659660339</v>
+        <v>0.261</v>
       </c>
       <c r="EN4" t="n">
-        <v>0.5538958311080933</v>
+        <v>0.554</v>
       </c>
       <c r="EO4" t="n">
-        <v>0.1447798767941677</v>
+        <v>0.145</v>
       </c>
       <c r="EP4" t="inlineStr"/>
       <c r="EQ4" t="inlineStr"/>
@@ -3543,23 +3499,21 @@
       <c r="FB4" t="inlineStr"/>
       <c r="FC4" t="inlineStr"/>
       <c r="FD4" t="inlineStr"/>
-      <c r="FE4" t="n">
-        <v>0.0001646030432311818</v>
-      </c>
+      <c r="FE4" t="inlineStr"/>
       <c r="FF4" t="n">
-        <v>0.450204998254776</v>
+        <v>0.45</v>
       </c>
       <c r="FG4" t="n">
-        <v>7.410511279062502e-05</v>
+        <v>0</v>
       </c>
       <c r="FH4" t="n">
-        <v>0.006520747672766447</v>
+        <v>0.007</v>
       </c>
       <c r="FI4" t="n">
-        <v>0.4451948404312134</v>
+        <v>0.445</v>
       </c>
       <c r="FJ4" t="n">
-        <v>0.002903003219669464</v>
+        <v>0.003</v>
       </c>
       <c r="FK4" t="inlineStr"/>
       <c r="FL4" t="inlineStr"/>
@@ -3568,13 +3522,13 @@
       <c r="FO4" t="inlineStr"/>
       <c r="FP4" t="inlineStr"/>
       <c r="FQ4" t="n">
-        <v>0.02727514877915382</v>
+        <v>0.027</v>
       </c>
       <c r="FR4" t="n">
-        <v>0.4432053565979004</v>
+        <v>0.443</v>
       </c>
       <c r="FS4" t="n">
-        <v>0.01208849204092566</v>
+        <v>0.012</v>
       </c>
       <c r="FT4" t="inlineStr"/>
       <c r="FU4" t="inlineStr"/>
@@ -3591,32 +3545,28 @@
       <c r="GF4" t="inlineStr"/>
       <c r="GG4" t="inlineStr"/>
       <c r="GH4" t="inlineStr"/>
-      <c r="GI4" t="n">
-        <v>0.0001525892730569467</v>
-      </c>
+      <c r="GI4" t="inlineStr"/>
       <c r="GJ4" t="n">
-        <v>0.5591141581535339</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="GK4" t="n">
-        <v>8.531482294849447e-05</v>
+        <v>0</v>
       </c>
       <c r="GL4" t="n">
-        <v>0.9828148484230042</v>
+        <v>0.983</v>
       </c>
       <c r="GM4" t="n">
-        <v>0.5389822125434875</v>
+        <v>0.539</v>
       </c>
       <c r="GN4" t="n">
-        <v>0.5297197215236231</v>
-      </c>
-      <c r="GO4" t="n">
-        <v>0.0001566253049531952</v>
-      </c>
+        <v>0.53</v>
+      </c>
+      <c r="GO4" t="inlineStr"/>
       <c r="GP4" t="n">
-        <v>0.5185633301734924</v>
+        <v>0.519</v>
       </c>
       <c r="GQ4" t="n">
-        <v>8.122013972596768e-05</v>
+        <v>0</v>
       </c>
       <c r="GR4" t="inlineStr"/>
       <c r="GS4" t="inlineStr"/>
@@ -3624,53 +3574,43 @@
       <c r="GU4" t="inlineStr"/>
       <c r="GV4" t="inlineStr"/>
       <c r="GW4" t="inlineStr"/>
-      <c r="GX4" t="n">
-        <v>0.0001501683873357251</v>
-      </c>
+      <c r="GX4" t="inlineStr"/>
       <c r="GY4" t="n">
-        <v>0.4699337780475616</v>
+        <v>0.47</v>
       </c>
       <c r="GZ4" t="n">
-        <v>7.056919760398692e-05</v>
-      </c>
-      <c r="HA4" t="n">
-        <v>0.0001618287060409784</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="HA4" t="inlineStr"/>
       <c r="HB4" t="n">
-        <v>0.5037731528282166</v>
+        <v>0.504</v>
       </c>
       <c r="HC4" t="n">
-        <v>8.152495746037436e-05</v>
-      </c>
-      <c r="HD4" t="n">
-        <v>0.0001618287060409784</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="HD4" t="inlineStr"/>
       <c r="HE4" t="n">
-        <v>0.5037731528282166</v>
+        <v>0.504</v>
       </c>
       <c r="HF4" t="n">
-        <v>8.152495746037436e-05</v>
-      </c>
-      <c r="HG4" t="n">
-        <v>0.0001618288515601307</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="HG4" t="inlineStr"/>
       <c r="HH4" t="n">
-        <v>0.5037731528282166</v>
+        <v>0.504</v>
       </c>
       <c r="HI4" t="n">
-        <v>8.15250307690165e-05</v>
+        <v>0</v>
       </c>
       <c r="HJ4" t="inlineStr"/>
       <c r="HK4" t="inlineStr"/>
       <c r="HL4" t="inlineStr"/>
-      <c r="HM4" t="n">
-        <v>0.0001506886328570545</v>
-      </c>
+      <c r="HM4" t="inlineStr"/>
       <c r="HN4" t="n">
-        <v>0.5719701051712036</v>
+        <v>0.572</v>
       </c>
       <c r="HO4" t="n">
-        <v>8.618939318335433e-05</v>
+        <v>0</v>
       </c>
       <c r="HP4" t="inlineStr"/>
       <c r="HQ4" t="inlineStr"/>
@@ -3684,50 +3624,40 @@
       <c r="HY4" t="inlineStr"/>
       <c r="HZ4" t="inlineStr"/>
       <c r="IA4" t="inlineStr"/>
-      <c r="IB4" t="n">
-        <v>0.0003275040362495929</v>
-      </c>
+      <c r="IB4" t="inlineStr"/>
       <c r="IC4" t="n">
-        <v>0.690001904964447</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="ID4" t="n">
-        <v>0.0002259784088957644</v>
-      </c>
-      <c r="IE4" t="n">
-        <v>0.0001572838227730244</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="IE4" t="inlineStr"/>
       <c r="IF4" t="n">
-        <v>0.4829238951206207</v>
+        <v>0.483</v>
       </c>
       <c r="IG4" t="n">
-        <v>7.595611633301035e-05</v>
-      </c>
-      <c r="IH4" t="n">
-        <v>0.0001586403086548671</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="IH4" t="inlineStr"/>
       <c r="II4" t="n">
-        <v>0.4961367249488831</v>
+        <v>0.496</v>
       </c>
       <c r="IJ4" t="n">
-        <v>7.870728318090572e-05</v>
-      </c>
-      <c r="IK4" t="n">
-        <v>0.0001606599107617512</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="IK4" t="inlineStr"/>
       <c r="IL4" t="n">
-        <v>0.5000433325767517</v>
+        <v>0.5</v>
       </c>
       <c r="IM4" t="n">
-        <v>8.033691718878962e-05</v>
-      </c>
-      <c r="IN4" t="n">
-        <v>0.0003455314435996115</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="IN4" t="inlineStr"/>
       <c r="IO4" t="n">
-        <v>0.5281539559364319</v>
+        <v>0.528</v>
       </c>
       <c r="IP4" t="n">
-        <v>0.0001824937988375609</v>
+        <v>0</v>
       </c>
       <c r="IQ4" t="inlineStr"/>
       <c r="IR4" t="inlineStr"/>
@@ -3735,38 +3665,32 @@
       <c r="IT4" t="inlineStr"/>
       <c r="IU4" t="inlineStr"/>
       <c r="IV4" t="inlineStr"/>
-      <c r="IW4" t="n">
-        <v>0.0001593558845343068</v>
-      </c>
+      <c r="IW4" t="inlineStr"/>
       <c r="IX4" t="n">
-        <v>0.5053677558898926</v>
+        <v>0.505</v>
       </c>
       <c r="IY4" t="n">
-        <v>8.053332575495148e-05</v>
+        <v>0</v>
       </c>
       <c r="IZ4" t="inlineStr"/>
       <c r="JA4" t="inlineStr"/>
       <c r="JB4" t="inlineStr"/>
-      <c r="JC4" t="n">
-        <v>0.0001594400964677334</v>
-      </c>
+      <c r="JC4" t="inlineStr"/>
       <c r="JD4" t="n">
-        <v>0.5210622549057007</v>
+        <v>0.521</v>
       </c>
       <c r="JE4" t="n">
-        <v>8.30782161878596e-05</v>
+        <v>0</v>
       </c>
       <c r="JF4" t="inlineStr"/>
       <c r="JG4" t="inlineStr"/>
       <c r="JH4" t="inlineStr"/>
-      <c r="JI4" t="n">
-        <v>0.0003461460000835359</v>
-      </c>
+      <c r="JI4" t="inlineStr"/>
       <c r="JJ4" t="n">
-        <v>0.4979675114154816</v>
+        <v>0.498</v>
       </c>
       <c r="JK4" t="n">
-        <v>0.0001723694622480215</v>
+        <v>0</v>
       </c>
       <c r="JL4" t="inlineStr"/>
       <c r="JM4" t="inlineStr"/>
@@ -3777,32 +3701,28 @@
       <c r="JR4" t="inlineStr"/>
       <c r="JS4" t="inlineStr"/>
       <c r="JT4" t="inlineStr"/>
-      <c r="JU4" t="n">
-        <v>0.0003254525654483587</v>
-      </c>
+      <c r="JU4" t="inlineStr"/>
       <c r="JV4" t="n">
-        <v>0.4746384024620056</v>
+        <v>0.475</v>
       </c>
       <c r="JW4" t="n">
-        <v>0.0001544722857415703</v>
-      </c>
-      <c r="JX4" t="n">
-        <v>0.0002290773409185931</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="JX4" t="inlineStr"/>
       <c r="JY4" t="n">
-        <v>0.4748465120792389</v>
+        <v>0.475</v>
       </c>
       <c r="JZ4" t="n">
-        <v>0.0001087765763315806</v>
+        <v>0</v>
       </c>
       <c r="KA4" t="n">
-        <v>0.9787035584449768</v>
+        <v>0.979</v>
       </c>
       <c r="KB4" t="n">
-        <v>0.5901048183441162</v>
+        <v>0.59</v>
       </c>
       <c r="KC4" t="n">
-        <v>0.5775376855689132</v>
+        <v>0.578</v>
       </c>
       <c r="KD4" t="inlineStr"/>
       <c r="KE4" t="inlineStr"/>
@@ -3811,13 +3731,13 @@
       <c r="KH4" t="inlineStr"/>
       <c r="KI4" t="inlineStr"/>
       <c r="KJ4" t="n">
-        <v>0.0006676302873529494</v>
+        <v>0.001</v>
       </c>
       <c r="KK4" t="n">
-        <v>0.3389908075332642</v>
+        <v>0.339</v>
       </c>
       <c r="KL4" t="n">
-        <v>0.0002263205302434415</v>
+        <v>0</v>
       </c>
       <c r="KM4" t="inlineStr"/>
       <c r="KN4" t="inlineStr"/>
@@ -3840,14 +3760,12 @@
       <c r="LE4" t="inlineStr"/>
       <c r="LF4" t="inlineStr"/>
       <c r="LG4" t="inlineStr"/>
-      <c r="LH4" t="n">
-        <v>0.000243519913055934</v>
-      </c>
+      <c r="LH4" t="inlineStr"/>
       <c r="LI4" t="n">
-        <v>0.3114631474018097</v>
+        <v>0.311</v>
       </c>
       <c r="LJ4" t="n">
-        <v>7.584747857541626e-05</v>
+        <v>0</v>
       </c>
       <c r="LK4" t="inlineStr"/>
       <c r="LL4" t="inlineStr"/>
@@ -3869,34 +3787,32 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>0.0006583424983546138</v>
+        <v>0.001</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4537066221237183</v>
+        <v>0.454</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0002986943511289614</v>
+        <v>0</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
-        <v>0.9922088384628296</v>
+        <v>0.992</v>
       </c>
       <c r="L5" t="n">
-        <v>0.4826338589191437</v>
+        <v>0.483</v>
       </c>
       <c r="M5" t="n">
-        <v>0.4788735805609967</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.0001009869301924482</v>
-      </c>
+        <v>0.479</v>
+      </c>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>0.496182382106781</v>
+        <v>0.496</v>
       </c>
       <c r="P5" t="n">
-        <v>5.010793558454015e-05</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
@@ -3917,13 +3833,13 @@
       <c r="AG5" t="inlineStr"/>
       <c r="AH5" t="inlineStr"/>
       <c r="AI5" t="n">
-        <v>0.00105688814073801</v>
+        <v>0.001</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.500852108001709</v>
+        <v>0.501</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.0005293446532106394</v>
+        <v>0.001</v>
       </c>
       <c r="AL5" t="inlineStr"/>
       <c r="AM5" t="inlineStr"/>
@@ -3989,13 +3905,13 @@
       <c r="CU5" t="inlineStr"/>
       <c r="CV5" t="inlineStr"/>
       <c r="CW5" t="n">
-        <v>0.9109261631965637</v>
+        <v>0.911</v>
       </c>
       <c r="CX5" t="n">
-        <v>0.4346454739570618</v>
+        <v>0.435</v>
       </c>
       <c r="CY5" t="n">
-        <v>0.3959299339424582</v>
+        <v>0.396</v>
       </c>
       <c r="CZ5" t="inlineStr"/>
       <c r="DA5" t="inlineStr"/>
@@ -4015,41 +3931,33 @@
       <c r="DO5" t="inlineStr"/>
       <c r="DP5" t="inlineStr"/>
       <c r="DQ5" t="inlineStr"/>
-      <c r="DR5" t="n">
-        <v>0.0001001709388219751</v>
-      </c>
+      <c r="DR5" t="inlineStr"/>
       <c r="DS5" t="n">
-        <v>0.4549297392368317</v>
+        <v>0.455</v>
       </c>
       <c r="DT5" t="n">
-        <v>4.557073907738977e-05</v>
-      </c>
-      <c r="DU5" t="n">
-        <v>0.0001013895816868171</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="DU5" t="inlineStr"/>
       <c r="DV5" t="n">
-        <v>0.4725372195243835</v>
+        <v>0.473</v>
       </c>
       <c r="DW5" t="n">
-        <v>4.791035101902891e-05</v>
-      </c>
-      <c r="DX5" t="n">
-        <v>0.000147354046930559</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="DX5" t="inlineStr"/>
       <c r="DY5" t="n">
-        <v>0.3610756993293762</v>
+        <v>0.361</v>
       </c>
       <c r="DZ5" t="n">
-        <v>5.320596554446531e-05</v>
-      </c>
-      <c r="EA5" t="n">
-        <v>0.0001018969851429574</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="EA5" t="inlineStr"/>
       <c r="EB5" t="n">
-        <v>0.5744572877883911</v>
+        <v>0.574</v>
       </c>
       <c r="EC5" t="n">
-        <v>5.85354657190373e-05</v>
+        <v>0</v>
       </c>
       <c r="ED5" t="inlineStr"/>
       <c r="EE5" t="inlineStr"/>
@@ -4063,23 +3971,21 @@
       <c r="EM5" t="inlineStr"/>
       <c r="EN5" t="inlineStr"/>
       <c r="EO5" t="inlineStr"/>
-      <c r="EP5" t="n">
-        <v>0.0001466836692998186</v>
-      </c>
+      <c r="EP5" t="inlineStr"/>
       <c r="EQ5" t="n">
-        <v>0.5203027129173279</v>
+        <v>0.52</v>
       </c>
       <c r="ER5" t="n">
-        <v>7.631991107736377e-05</v>
+        <v>0</v>
       </c>
       <c r="ES5" t="n">
-        <v>0.001145511749200523</v>
+        <v>0.001</v>
       </c>
       <c r="ET5" t="n">
-        <v>0.2942646741867065</v>
+        <v>0.294</v>
       </c>
       <c r="EU5" t="n">
-        <v>0.0003370836416555362</v>
+        <v>0</v>
       </c>
       <c r="EV5" t="inlineStr"/>
       <c r="EW5" t="inlineStr"/>
@@ -4099,14 +4005,12 @@
       <c r="FK5" t="inlineStr"/>
       <c r="FL5" t="inlineStr"/>
       <c r="FM5" t="inlineStr"/>
-      <c r="FN5" t="n">
-        <v>9.85886508715339e-05</v>
-      </c>
+      <c r="FN5" t="inlineStr"/>
       <c r="FO5" t="n">
-        <v>0.3102152645587921</v>
+        <v>0.31</v>
       </c>
       <c r="FP5" t="n">
-        <v>3.058370441260728e-05</v>
+        <v>0</v>
       </c>
       <c r="FQ5" t="inlineStr"/>
       <c r="FR5" t="inlineStr"/>
@@ -4115,13 +4019,13 @@
       <c r="FU5" t="inlineStr"/>
       <c r="FV5" t="inlineStr"/>
       <c r="FW5" t="n">
-        <v>0.0005975591484457254</v>
+        <v>0.001</v>
       </c>
       <c r="FX5" t="n">
-        <v>0.4024854004383087</v>
+        <v>0.402</v>
       </c>
       <c r="FY5" t="n">
-        <v>0.0002405088331477526</v>
+        <v>0</v>
       </c>
       <c r="FZ5" t="inlineStr"/>
       <c r="GA5" t="inlineStr"/>
@@ -4168,14 +4072,12 @@
       <c r="HP5" t="inlineStr"/>
       <c r="HQ5" t="inlineStr"/>
       <c r="HR5" t="inlineStr"/>
-      <c r="HS5" t="n">
-        <v>0.0001682829606579617</v>
-      </c>
+      <c r="HS5" t="inlineStr"/>
       <c r="HT5" t="n">
-        <v>0.5282847881317139</v>
+        <v>0.528</v>
       </c>
       <c r="HU5" t="n">
-        <v>8.890132821736882e-05</v>
+        <v>0</v>
       </c>
       <c r="HV5" t="inlineStr"/>
       <c r="HW5" t="inlineStr"/>
@@ -4222,23 +4124,19 @@
       <c r="JL5" t="inlineStr"/>
       <c r="JM5" t="inlineStr"/>
       <c r="JN5" t="inlineStr"/>
-      <c r="JO5" t="n">
-        <v>0.000176917455974035</v>
-      </c>
+      <c r="JO5" t="inlineStr"/>
       <c r="JP5" t="n">
-        <v>0.7265301942825317</v>
+        <v>0.727</v>
       </c>
       <c r="JQ5" t="n">
-        <v>0.0001285358736607869</v>
-      </c>
-      <c r="JR5" t="n">
-        <v>9.37940931180492e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="JR5" t="inlineStr"/>
       <c r="JS5" t="n">
-        <v>0.6976924538612366</v>
+        <v>0.698</v>
       </c>
       <c r="JT5" t="n">
-        <v>6.543943098522107e-05</v>
+        <v>0</v>
       </c>
       <c r="JU5" t="inlineStr"/>
       <c r="JV5" t="inlineStr"/>
@@ -4258,53 +4156,43 @@
       <c r="KJ5" t="inlineStr"/>
       <c r="KK5" t="inlineStr"/>
       <c r="KL5" t="inlineStr"/>
-      <c r="KM5" t="n">
-        <v>0.000132512956042774</v>
-      </c>
+      <c r="KM5" t="inlineStr"/>
       <c r="KN5" t="n">
-        <v>0.6321638822555542</v>
+        <v>0.632</v>
       </c>
       <c r="KO5" t="n">
-        <v>8.376990474115963e-05</v>
-      </c>
-      <c r="KP5" t="n">
-        <v>0.0001206323941005394</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="KP5" t="inlineStr"/>
       <c r="KQ5" t="n">
-        <v>0.6142929792404175</v>
+        <v>0.614</v>
       </c>
       <c r="KR5" t="n">
-        <v>7.41036327649245e-05</v>
-      </c>
-      <c r="KS5" t="n">
-        <v>0.0001847047678893432</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="KS5" t="inlineStr"/>
       <c r="KT5" t="n">
-        <v>0.6422749757766724</v>
+        <v>0.642</v>
       </c>
       <c r="KU5" t="n">
-        <v>0.0001186312503219638</v>
-      </c>
-      <c r="KV5" t="n">
-        <v>0.000143269426189363</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="KV5" t="inlineStr"/>
       <c r="KW5" t="n">
-        <v>0.5378153920173645</v>
+        <v>0.538</v>
       </c>
       <c r="KX5" t="n">
-        <v>7.705250261013513e-05</v>
+        <v>0</v>
       </c>
       <c r="KY5" t="inlineStr"/>
       <c r="KZ5" t="inlineStr"/>
       <c r="LA5" t="inlineStr"/>
-      <c r="LB5" t="n">
-        <v>0.0001341103197773919</v>
-      </c>
+      <c r="LB5" t="inlineStr"/>
       <c r="LC5" t="n">
-        <v>0.5290790796279907</v>
+        <v>0.529</v>
       </c>
       <c r="LD5" t="n">
-        <v>7.0954964556438e-05</v>
+        <v>0</v>
       </c>
       <c r="LE5" t="inlineStr"/>
       <c r="LF5" t="inlineStr"/>
@@ -4312,23 +4200,19 @@
       <c r="LH5" t="inlineStr"/>
       <c r="LI5" t="inlineStr"/>
       <c r="LJ5" t="inlineStr"/>
-      <c r="LK5" t="n">
-        <v>0.0001206838132929988</v>
-      </c>
+      <c r="LK5" t="inlineStr"/>
       <c r="LL5" t="n">
-        <v>0.4065775275230408</v>
+        <v>0.407</v>
       </c>
       <c r="LM5" t="n">
-        <v>4.906732642071974e-05</v>
-      </c>
-      <c r="LN5" t="n">
-        <v>9.736372157931328e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="LN5" t="inlineStr"/>
       <c r="LO5" t="n">
-        <v>0.5199026465415955</v>
+        <v>0.52</v>
       </c>
       <c r="LP5" t="n">
-        <v>5.061965652622402e-05</v>
+        <v>0</v>
       </c>
       <c r="LQ5" t="inlineStr"/>
       <c r="LR5" t="inlineStr"/>
@@ -4359,13 +4243,13 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="n">
-        <v>0.8980154991149902</v>
+        <v>0.898</v>
       </c>
       <c r="U6" t="n">
-        <v>0.3474219739437103</v>
+        <v>0.347</v>
       </c>
       <c r="V6" t="n">
-        <v>0.3119903173345762</v>
+        <v>0.312</v>
       </c>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
@@ -4376,14 +4260,12 @@
       <c r="AC6" t="inlineStr"/>
       <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="n">
-        <v>0.0002047236630460247</v>
-      </c>
+      <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="n">
-        <v>0.3337576687335968</v>
+        <v>0.334</v>
       </c>
       <c r="AH6" t="n">
-        <v>6.832809251284362e-05</v>
+        <v>0</v>
       </c>
       <c r="AI6" t="inlineStr"/>
       <c r="AJ6" t="inlineStr"/>
@@ -4392,133 +4274,125 @@
       <c r="AM6" t="inlineStr"/>
       <c r="AN6" t="inlineStr"/>
       <c r="AO6" t="n">
-        <v>0.001373584731481969</v>
+        <v>0.001</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.34035524725914</v>
+        <v>0.34</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.0004675067709149251</v>
+        <v>0</v>
       </c>
       <c r="AR6" t="n">
-        <v>0.002509616315364838</v>
+        <v>0.003</v>
       </c>
       <c r="AS6" t="n">
-        <v>0.3422820866107941</v>
+        <v>0.342</v>
       </c>
       <c r="AT6" t="n">
-        <v>0.0008589967090155692</v>
+        <v>0.001</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.001003099489025772</v>
+        <v>0.001</v>
       </c>
       <c r="AV6" t="n">
-        <v>0.3994565010070801</v>
+        <v>0.399</v>
       </c>
       <c r="AW6" t="n">
-        <v>0.0004006946120482247</v>
+        <v>0</v>
       </c>
       <c r="AX6" t="n">
-        <v>0.002866727765649557</v>
+        <v>0.003</v>
       </c>
       <c r="AY6" t="n">
-        <v>0.3321973085403442</v>
+        <v>0.332</v>
       </c>
       <c r="AZ6" t="n">
-        <v>0.0009523192480666576</v>
+        <v>0.001</v>
       </c>
       <c r="BA6" t="n">
-        <v>0.004900973755866289</v>
+        <v>0.005</v>
       </c>
       <c r="BB6" t="n">
-        <v>0.3289389312267303</v>
+        <v>0.329</v>
       </c>
       <c r="BC6" t="n">
-        <v>0.001612121069224912</v>
+        <v>0.002</v>
       </c>
       <c r="BD6" t="inlineStr"/>
       <c r="BE6" t="inlineStr"/>
       <c r="BF6" t="inlineStr"/>
       <c r="BG6" t="n">
-        <v>0.0006629080744460225</v>
+        <v>0.001</v>
       </c>
       <c r="BH6" t="n">
-        <v>0.3433867394924164</v>
+        <v>0.343</v>
       </c>
       <c r="BI6" t="n">
-        <v>0.0002276338422672157</v>
+        <v>0</v>
       </c>
       <c r="BJ6" t="n">
-        <v>0.0005372412852011621</v>
+        <v>0.001</v>
       </c>
       <c r="BK6" t="n">
-        <v>0.4055239260196686</v>
+        <v>0.406</v>
       </c>
       <c r="BL6" t="n">
-        <v>0.0002178641951946277</v>
-      </c>
-      <c r="BM6" t="n">
-        <v>0.000478965463116765</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="BM6" t="inlineStr"/>
       <c r="BN6" t="n">
-        <v>0.4085825681686401</v>
+        <v>0.409</v>
       </c>
       <c r="BO6" t="n">
-        <v>0.0001956969389843299</v>
+        <v>0</v>
       </c>
       <c r="BP6" t="n">
-        <v>0.0005349528510123491</v>
+        <v>0.001</v>
       </c>
       <c r="BQ6" t="n">
-        <v>0.3387523293495178</v>
+        <v>0.339</v>
       </c>
       <c r="BR6" t="n">
-        <v>0.0001812165243725988</v>
+        <v>0</v>
       </c>
       <c r="BS6" t="n">
-        <v>0.7463898062705994</v>
+        <v>0.746</v>
       </c>
       <c r="BT6" t="n">
-        <v>0.356881320476532</v>
+        <v>0.357</v>
       </c>
       <c r="BU6" t="n">
-        <v>0.2663725796520744</v>
-      </c>
-      <c r="BV6" t="n">
-        <v>0.000384246843168512</v>
-      </c>
+        <v>0.266</v>
+      </c>
+      <c r="BV6" t="inlineStr"/>
       <c r="BW6" t="n">
-        <v>0.3212482333183289</v>
+        <v>0.321</v>
       </c>
       <c r="BX6" t="n">
-        <v>0.0001234386195260295</v>
+        <v>0</v>
       </c>
       <c r="BY6" t="n">
-        <v>0.8598341941833496</v>
+        <v>0.86</v>
       </c>
       <c r="BZ6" t="n">
-        <v>0.3533122539520264</v>
+        <v>0.353</v>
       </c>
       <c r="CA6" t="n">
-        <v>0.3037899571719436</v>
-      </c>
-      <c r="CB6" t="n">
-        <v>0.0002255752333439887</v>
-      </c>
+        <v>0.304</v>
+      </c>
+      <c r="CB6" t="inlineStr"/>
       <c r="CC6" t="n">
-        <v>0.3403876125812531</v>
+        <v>0.34</v>
       </c>
       <c r="CD6" t="n">
-        <v>7.678301513541937e-05</v>
-      </c>
-      <c r="CE6" t="n">
-        <v>0.0001886828249553218</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="CE6" t="inlineStr"/>
       <c r="CF6" t="n">
-        <v>0.3434313237667084</v>
+        <v>0.343</v>
       </c>
       <c r="CG6" t="n">
-        <v>6.47995923464483e-05</v>
+        <v>0</v>
       </c>
       <c r="CH6" t="inlineStr"/>
       <c r="CI6" t="inlineStr"/>
@@ -4526,23 +4400,19 @@
       <c r="CK6" t="inlineStr"/>
       <c r="CL6" t="inlineStr"/>
       <c r="CM6" t="inlineStr"/>
-      <c r="CN6" t="n">
-        <v>0.0001981645618798211</v>
-      </c>
+      <c r="CN6" t="inlineStr"/>
       <c r="CO6" t="n">
-        <v>0.4104751348495483</v>
+        <v>0.41</v>
       </c>
       <c r="CP6" t="n">
-        <v>8.134162526002124e-05</v>
-      </c>
-      <c r="CQ6" t="n">
-        <v>0.0001956172345671803</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="CQ6" t="inlineStr"/>
       <c r="CR6" t="n">
-        <v>0.4133908450603485</v>
+        <v>0.413</v>
       </c>
       <c r="CS6" t="n">
-        <v>8.086637390609507e-05</v>
+        <v>0</v>
       </c>
       <c r="CT6" t="inlineStr"/>
       <c r="CU6" t="inlineStr"/>
@@ -4562,14 +4432,12 @@
       <c r="DI6" t="inlineStr"/>
       <c r="DJ6" t="inlineStr"/>
       <c r="DK6" t="inlineStr"/>
-      <c r="DL6" t="n">
-        <v>0.0001668368931859732</v>
-      </c>
+      <c r="DL6" t="inlineStr"/>
       <c r="DM6" t="n">
-        <v>0.3340395987033844</v>
+        <v>0.334</v>
       </c>
       <c r="DN6" t="n">
-        <v>5.573012884876188e-05</v>
+        <v>0</v>
       </c>
       <c r="DO6" t="inlineStr"/>
       <c r="DP6" t="inlineStr"/>
@@ -4586,26 +4454,24 @@
       <c r="EA6" t="inlineStr"/>
       <c r="EB6" t="inlineStr"/>
       <c r="EC6" t="inlineStr"/>
-      <c r="ED6" t="n">
-        <v>0.0002301974745932966</v>
-      </c>
+      <c r="ED6" t="inlineStr"/>
       <c r="EE6" t="n">
-        <v>0.3343814015388489</v>
+        <v>0.334</v>
       </c>
       <c r="EF6" t="n">
-        <v>7.697375418521009e-05</v>
+        <v>0</v>
       </c>
       <c r="EG6" t="inlineStr"/>
       <c r="EH6" t="inlineStr"/>
       <c r="EI6" t="inlineStr"/>
       <c r="EJ6" t="n">
-        <v>0.06581370532512665</v>
+        <v>0.066</v>
       </c>
       <c r="EK6" t="n">
-        <v>0.3373047411441803</v>
+        <v>0.337</v>
       </c>
       <c r="EL6" t="n">
-        <v>0.0221992748384312</v>
+        <v>0.022</v>
       </c>
       <c r="EM6" t="inlineStr"/>
       <c r="EN6" t="inlineStr"/>
@@ -4620,13 +4486,13 @@
       <c r="EW6" t="inlineStr"/>
       <c r="EX6" t="inlineStr"/>
       <c r="EY6" t="n">
-        <v>0.0006471410160884261</v>
+        <v>0.001</v>
       </c>
       <c r="EZ6" t="n">
-        <v>0.3522735238075256</v>
+        <v>0.352</v>
       </c>
       <c r="FA6" t="n">
-        <v>0.0002279706461378525</v>
+        <v>0</v>
       </c>
       <c r="FB6" t="inlineStr"/>
       <c r="FC6" t="inlineStr"/>
@@ -4637,14 +4503,12 @@
       <c r="FH6" t="inlineStr"/>
       <c r="FI6" t="inlineStr"/>
       <c r="FJ6" t="inlineStr"/>
-      <c r="FK6" t="n">
-        <v>0.0002172780368709937</v>
-      </c>
+      <c r="FK6" t="inlineStr"/>
       <c r="FL6" t="n">
-        <v>0.3441546559333801</v>
+        <v>0.344</v>
       </c>
       <c r="FM6" t="n">
-        <v>7.477724802121711e-05</v>
+        <v>0</v>
       </c>
       <c r="FN6" t="inlineStr"/>
       <c r="FO6" t="inlineStr"/>
@@ -4653,13 +4517,13 @@
       <c r="FR6" t="inlineStr"/>
       <c r="FS6" t="inlineStr"/>
       <c r="FT6" t="n">
-        <v>0.003891039406880736</v>
+        <v>0.004</v>
       </c>
       <c r="FU6" t="n">
-        <v>0.3727795779705048</v>
+        <v>0.373</v>
       </c>
       <c r="FV6" t="n">
-        <v>0.001450500027963604</v>
+        <v>0.001</v>
       </c>
       <c r="FW6" t="inlineStr"/>
       <c r="FX6" t="inlineStr"/>
@@ -4667,23 +4531,19 @@
       <c r="FZ6" t="inlineStr"/>
       <c r="GA6" t="inlineStr"/>
       <c r="GB6" t="inlineStr"/>
-      <c r="GC6" t="n">
-        <v>0.0002055400400422513</v>
-      </c>
+      <c r="GC6" t="inlineStr"/>
       <c r="GD6" t="n">
-        <v>0.3201825320720673</v>
+        <v>0.32</v>
       </c>
       <c r="GE6" t="n">
-        <v>6.581033046292213e-05</v>
-      </c>
-      <c r="GF6" t="n">
-        <v>0.0002054085780400783</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="GF6" t="inlineStr"/>
       <c r="GG6" t="n">
-        <v>0.3461759388446808</v>
+        <v>0.346</v>
       </c>
       <c r="GH6" t="n">
-        <v>7.110750734977498e-05</v>
+        <v>0</v>
       </c>
       <c r="GI6" t="inlineStr"/>
       <c r="GJ6" t="inlineStr"/>
@@ -4694,23 +4554,21 @@
       <c r="GO6" t="inlineStr"/>
       <c r="GP6" t="inlineStr"/>
       <c r="GQ6" t="inlineStr"/>
-      <c r="GR6" t="n">
-        <v>0.0002290832344442606</v>
-      </c>
+      <c r="GR6" t="inlineStr"/>
       <c r="GS6" t="n">
-        <v>0.3505792617797852</v>
+        <v>0.351</v>
       </c>
       <c r="GT6" t="n">
-        <v>8.031183121759433e-05</v>
+        <v>0</v>
       </c>
       <c r="GU6" t="n">
-        <v>0.0006511673564091325</v>
+        <v>0.001</v>
       </c>
       <c r="GV6" t="n">
-        <v>0.3292534351348877</v>
+        <v>0.329</v>
       </c>
       <c r="GW6" t="n">
-        <v>0.0002143990889454106</v>
+        <v>0</v>
       </c>
       <c r="GX6" t="inlineStr"/>
       <c r="GY6" t="inlineStr"/>
@@ -4724,26 +4582,22 @@
       <c r="HG6" t="inlineStr"/>
       <c r="HH6" t="inlineStr"/>
       <c r="HI6" t="inlineStr"/>
-      <c r="HJ6" t="n">
-        <v>0.0001602503325557336</v>
-      </c>
+      <c r="HJ6" t="inlineStr"/>
       <c r="HK6" t="n">
-        <v>0.3228981792926788</v>
+        <v>0.323</v>
       </c>
       <c r="HL6" t="n">
-        <v>5.174454061329268e-05</v>
+        <v>0</v>
       </c>
       <c r="HM6" t="inlineStr"/>
       <c r="HN6" t="inlineStr"/>
       <c r="HO6" t="inlineStr"/>
-      <c r="HP6" t="n">
-        <v>0.0001883344812085852</v>
-      </c>
+      <c r="HP6" t="inlineStr"/>
       <c r="HQ6" t="n">
-        <v>0.3380043804645538</v>
+        <v>0.338</v>
       </c>
       <c r="HR6" t="n">
-        <v>6.3657879641021e-05</v>
+        <v>0</v>
       </c>
       <c r="HS6" t="inlineStr"/>
       <c r="HT6" t="inlineStr"/>
@@ -4784,26 +4638,22 @@
       <c r="JC6" t="inlineStr"/>
       <c r="JD6" t="inlineStr"/>
       <c r="JE6" t="inlineStr"/>
-      <c r="JF6" t="n">
-        <v>0.0003621490905061364</v>
-      </c>
+      <c r="JF6" t="inlineStr"/>
       <c r="JG6" t="n">
-        <v>0.3476216793060303</v>
+        <v>0.348</v>
       </c>
       <c r="JH6" t="n">
-        <v>0.0001258908750008947</v>
+        <v>0</v>
       </c>
       <c r="JI6" t="inlineStr"/>
       <c r="JJ6" t="inlineStr"/>
       <c r="JK6" t="inlineStr"/>
-      <c r="JL6" t="n">
-        <v>0.000184295407962054</v>
-      </c>
+      <c r="JL6" t="inlineStr"/>
       <c r="JM6" t="n">
-        <v>0.3334830701351166</v>
+        <v>0.333</v>
       </c>
       <c r="JN6" t="n">
-        <v>6.145939845898958e-05</v>
+        <v>0</v>
       </c>
       <c r="JO6" t="inlineStr"/>
       <c r="JP6" t="inlineStr"/>
@@ -4823,14 +4673,12 @@
       <c r="KD6" t="inlineStr"/>
       <c r="KE6" t="inlineStr"/>
       <c r="KF6" t="inlineStr"/>
-      <c r="KG6" t="n">
-        <v>0.000216943517443724</v>
-      </c>
+      <c r="KG6" t="inlineStr"/>
       <c r="KH6" t="n">
-        <v>0.3473349809646606</v>
+        <v>0.347</v>
       </c>
       <c r="KI6" t="n">
-        <v>7.535207250172239e-05</v>
+        <v>0</v>
       </c>
       <c r="KJ6" t="inlineStr"/>
       <c r="KK6" t="inlineStr"/>
@@ -4848,13 +4696,13 @@
       <c r="KW6" t="inlineStr"/>
       <c r="KX6" t="inlineStr"/>
       <c r="KY6" t="n">
-        <v>0.01484866626560688</v>
+        <v>0.015</v>
       </c>
       <c r="KZ6" t="n">
-        <v>0.3524650633335114</v>
+        <v>0.352</v>
       </c>
       <c r="LA6" t="n">
-        <v>0.005233636095725303</v>
+        <v>0.005</v>
       </c>
       <c r="LB6" t="inlineStr"/>
       <c r="LC6" t="inlineStr"/>
@@ -4897,25 +4745,25 @@
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="n">
-        <v>0.5779632925987244</v>
+        <v>0.578</v>
       </c>
       <c r="R7" t="n">
-        <v>0.1849659532308578</v>
+        <v>0.185</v>
       </c>
       <c r="S7" t="n">
-        <v>0.1069035313479683</v>
+        <v>0.107</v>
       </c>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="n">
-        <v>0.48979252576828</v>
+        <v>0.49</v>
       </c>
       <c r="X7" t="n">
-        <v>0.2298624664545059</v>
+        <v>0.23</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.112584918024079</v>
+        <v>0.113</v>
       </c>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
@@ -4948,13 +4796,13 @@
       <c r="BB7" t="inlineStr"/>
       <c r="BC7" t="inlineStr"/>
       <c r="BD7" t="n">
-        <v>0.05880988389253616</v>
+        <v>0.059</v>
       </c>
       <c r="BE7" t="n">
-        <v>0.2635025680065155</v>
+        <v>0.264</v>
       </c>
       <c r="BF7" t="n">
-        <v>0.01549655542984829</v>
+        <v>0.015</v>
       </c>
       <c r="BG7" t="inlineStr"/>
       <c r="BH7" t="inlineStr"/>
@@ -4996,13 +4844,13 @@
       <c r="CR7" t="inlineStr"/>
       <c r="CS7" t="inlineStr"/>
       <c r="CT7" t="n">
-        <v>0.1457740664482117</v>
+        <v>0.146</v>
       </c>
       <c r="CU7" t="n">
-        <v>0.1991849839687347</v>
+        <v>0.199</v>
       </c>
       <c r="CV7" t="n">
-        <v>0.02903600508854431</v>
+        <v>0.029</v>
       </c>
       <c r="CW7" t="inlineStr"/>
       <c r="CX7" t="inlineStr"/>
@@ -5017,13 +4865,13 @@
       <c r="DG7" t="inlineStr"/>
       <c r="DH7" t="inlineStr"/>
       <c r="DI7" t="n">
-        <v>0.3408040404319763</v>
+        <v>0.341</v>
       </c>
       <c r="DJ7" t="n">
-        <v>0.1935922354459763</v>
+        <v>0.194</v>
       </c>
       <c r="DK7" t="n">
-        <v>0.06597701603624717</v>
+        <v>0.066</v>
       </c>
       <c r="DL7" t="inlineStr"/>
       <c r="DM7" t="inlineStr"/>
@@ -5047,13 +4895,13 @@
       <c r="EE7" t="inlineStr"/>
       <c r="EF7" t="inlineStr"/>
       <c r="EG7" t="n">
-        <v>0.1200842335820198</v>
+        <v>0.12</v>
       </c>
       <c r="EH7" t="n">
-        <v>0.183757483959198</v>
+        <v>0.184</v>
       </c>
       <c r="EI7" t="n">
-        <v>0.02206637662620059</v>
+        <v>0.022</v>
       </c>
       <c r="EJ7" t="inlineStr"/>
       <c r="EK7" t="inlineStr"/>
@@ -5068,25 +4916,25 @@
       <c r="ET7" t="inlineStr"/>
       <c r="EU7" t="inlineStr"/>
       <c r="EV7" t="n">
-        <v>0.5422976613044739</v>
+        <v>0.542</v>
       </c>
       <c r="EW7" t="n">
-        <v>0.1869892179965973</v>
+        <v>0.187</v>
       </c>
       <c r="EX7" t="n">
-        <v>0.1014038156087071</v>
+        <v>0.101</v>
       </c>
       <c r="EY7" t="inlineStr"/>
       <c r="EZ7" t="inlineStr"/>
       <c r="FA7" t="inlineStr"/>
       <c r="FB7" t="n">
-        <v>0.5037320256233215</v>
+        <v>0.504</v>
       </c>
       <c r="FC7" t="n">
-        <v>0.1689972877502441</v>
+        <v>0.169</v>
       </c>
       <c r="FD7" t="n">
-        <v>0.08512934608327782</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="FE7" t="inlineStr"/>
       <c r="FF7" t="inlineStr"/>
@@ -5110,13 +4958,13 @@
       <c r="FX7" t="inlineStr"/>
       <c r="FY7" t="inlineStr"/>
       <c r="FZ7" t="n">
-        <v>0.08157650381326675</v>
+        <v>0.082</v>
       </c>
       <c r="GA7" t="n">
-        <v>0.1787657290697098</v>
+        <v>0.179</v>
       </c>
       <c r="GB7" t="n">
-        <v>0.01458308317913659</v>
+        <v>0.015</v>
       </c>
       <c r="GC7" t="inlineStr"/>
       <c r="GD7" t="inlineStr"/>
@@ -5164,22 +5012,22 @@
       <c r="HT7" t="inlineStr"/>
       <c r="HU7" t="inlineStr"/>
       <c r="HV7" t="n">
-        <v>0.03823705390095711</v>
+        <v>0.038</v>
       </c>
       <c r="HW7" t="n">
-        <v>0.1782007217407227</v>
+        <v>0.178</v>
       </c>
       <c r="HX7" t="n">
-        <v>0.006813870602389471</v>
+        <v>0.007</v>
       </c>
       <c r="HY7" t="n">
-        <v>0.02178427577018738</v>
+        <v>0.022</v>
       </c>
       <c r="HZ7" t="n">
-        <v>0.2073110938072205</v>
+        <v>0.207</v>
       </c>
       <c r="IA7" t="n">
-        <v>0.004516122037715675</v>
+        <v>0.005</v>
       </c>
       <c r="IB7" t="inlineStr"/>
       <c r="IC7" t="inlineStr"/>
@@ -5197,34 +5045,34 @@
       <c r="IO7" t="inlineStr"/>
       <c r="IP7" t="inlineStr"/>
       <c r="IQ7" t="n">
-        <v>0.1776786744594574</v>
+        <v>0.178</v>
       </c>
       <c r="IR7" t="n">
-        <v>0.193981260061264</v>
+        <v>0.194</v>
       </c>
       <c r="IS7" t="n">
-        <v>0.03446633315766068</v>
+        <v>0.034</v>
       </c>
       <c r="IT7" t="n">
-        <v>0.1286880522966385</v>
+        <v>0.129</v>
       </c>
       <c r="IU7" t="n">
-        <v>0.2028439193964005</v>
+        <v>0.203</v>
       </c>
       <c r="IV7" t="n">
-        <v>0.0261035889073391</v>
+        <v>0.026</v>
       </c>
       <c r="IW7" t="inlineStr"/>
       <c r="IX7" t="inlineStr"/>
       <c r="IY7" t="inlineStr"/>
       <c r="IZ7" t="n">
-        <v>0.14399254322052</v>
+        <v>0.144</v>
       </c>
       <c r="JA7" t="n">
-        <v>0.2036134451627731</v>
+        <v>0.204</v>
       </c>
       <c r="JB7" t="n">
-        <v>0.02931881780287959</v>
+        <v>0.029</v>
       </c>
       <c r="JC7" t="inlineStr"/>
       <c r="JD7" t="inlineStr"/>
@@ -5254,13 +5102,13 @@
       <c r="KB7" t="inlineStr"/>
       <c r="KC7" t="inlineStr"/>
       <c r="KD7" t="n">
-        <v>0.4312750995159149</v>
+        <v>0.431</v>
       </c>
       <c r="KE7" t="n">
-        <v>0.1839507967233658</v>
+        <v>0.184</v>
       </c>
       <c r="KF7" t="n">
-        <v>0.07933339816290141</v>
+        <v>0.079</v>
       </c>
       <c r="KG7" t="inlineStr"/>
       <c r="KH7" t="inlineStr"/>
@@ -5287,13 +5135,13 @@
       <c r="LC7" t="inlineStr"/>
       <c r="LD7" t="inlineStr"/>
       <c r="LE7" t="n">
-        <v>0.1359595954418182</v>
+        <v>0.136</v>
       </c>
       <c r="LF7" t="n">
-        <v>0.1711496114730835</v>
+        <v>0.171</v>
       </c>
       <c r="LG7" t="n">
-        <v>0.02326943193590481</v>
+        <v>0.023</v>
       </c>
       <c r="LH7" t="inlineStr"/>
       <c r="LI7" t="inlineStr"/>
@@ -5305,13 +5153,13 @@
       <c r="LO7" t="inlineStr"/>
       <c r="LP7" t="inlineStr"/>
       <c r="LQ7" t="n">
-        <v>0.0121166305616498</v>
+        <v>0.012</v>
       </c>
       <c r="LR7" t="n">
-        <v>0.1965609192848206</v>
+        <v>0.197</v>
       </c>
       <c r="LS7" t="n">
-        <v>0.002381656041832436</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="8">
@@ -5321,25 +5169,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01382946409285069</v>
+        <v>0.014</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5155474543571472</v>
+        <v>0.516</v>
       </c>
       <c r="D8" t="n">
-        <v>0.007129745008192745</v>
+        <v>0.007</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>0.0007112178136594594</v>
+        <v>0.001</v>
       </c>
       <c r="I8" t="n">
-        <v>0.6007758378982544</v>
+        <v>0.601</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0004272824779294263</v>
+        <v>0</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
@@ -5357,22 +5205,22 @@
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="n">
-        <v>0.008599394001066685</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.5111820101737976</v>
+        <v>0.511</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.004395855511741764</v>
+        <v>0.004</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.001665574149228632</v>
+        <v>0.002</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.4764658510684967</v>
+        <v>0.476</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.0007935892045299077</v>
+        <v>0.001</v>
       </c>
       <c r="AF8" t="inlineStr"/>
       <c r="AG8" t="inlineStr"/>
@@ -5381,13 +5229,13 @@
       <c r="AJ8" t="inlineStr"/>
       <c r="AK8" t="inlineStr"/>
       <c r="AL8" t="n">
-        <v>0.007859695702791214</v>
+        <v>0.008</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.2820135653018951</v>
+        <v>0.282</v>
       </c>
       <c r="AN8" t="n">
-        <v>0.002216540807332135</v>
+        <v>0.002</v>
       </c>
       <c r="AO8" t="inlineStr"/>
       <c r="AP8" t="inlineStr"/>
@@ -5434,23 +5282,19 @@
       <c r="CE8" t="inlineStr"/>
       <c r="CF8" t="inlineStr"/>
       <c r="CG8" t="inlineStr"/>
-      <c r="CH8" t="n">
-        <v>0.0004405386280268431</v>
-      </c>
+      <c r="CH8" t="inlineStr"/>
       <c r="CI8" t="n">
-        <v>0.5637864470481873</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="CJ8" t="n">
-        <v>0.0002483697078827368</v>
-      </c>
-      <c r="CK8" t="n">
-        <v>0.0004325815825723112</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="CK8" t="inlineStr"/>
       <c r="CL8" t="n">
-        <v>0.3713476061820984</v>
+        <v>0.371</v>
       </c>
       <c r="CM8" t="n">
-        <v>0.0001606381351666915</v>
+        <v>0</v>
       </c>
       <c r="CN8" t="inlineStr"/>
       <c r="CO8" t="inlineStr"/>
@@ -5465,31 +5309,29 @@
       <c r="CX8" t="inlineStr"/>
       <c r="CY8" t="inlineStr"/>
       <c r="CZ8" t="n">
-        <v>0.002543678274378181</v>
+        <v>0.003</v>
       </c>
       <c r="DA8" t="n">
-        <v>0.3971855044364929</v>
+        <v>0.397</v>
       </c>
       <c r="DB8" t="n">
-        <v>0.001010312138533045</v>
-      </c>
-      <c r="DC8" t="n">
-        <v>0.0003465414047241211</v>
-      </c>
+        <v>0.001</v>
+      </c>
+      <c r="DC8" t="inlineStr"/>
       <c r="DD8" t="n">
-        <v>0.5865025520324707</v>
+        <v>0.587</v>
       </c>
       <c r="DE8" t="n">
-        <v>0.0002032474182556143</v>
+        <v>0</v>
       </c>
       <c r="DF8" t="n">
-        <v>0.002477099886164069</v>
+        <v>0.002</v>
       </c>
       <c r="DG8" t="n">
-        <v>0.5517855286598206</v>
+        <v>0.552</v>
       </c>
       <c r="DH8" t="n">
-        <v>0.001366827870230222</v>
+        <v>0.001</v>
       </c>
       <c r="DI8" t="inlineStr"/>
       <c r="DJ8" t="inlineStr"/>
@@ -5497,14 +5339,12 @@
       <c r="DL8" t="inlineStr"/>
       <c r="DM8" t="inlineStr"/>
       <c r="DN8" t="inlineStr"/>
-      <c r="DO8" t="n">
-        <v>0.0003444235771894455</v>
-      </c>
+      <c r="DO8" t="inlineStr"/>
       <c r="DP8" t="n">
-        <v>0.6274272203445435</v>
+        <v>0.627</v>
       </c>
       <c r="DQ8" t="n">
-        <v>0.0002161007276570981</v>
+        <v>0</v>
       </c>
       <c r="DR8" t="inlineStr"/>
       <c r="DS8" t="inlineStr"/>
@@ -5527,14 +5367,12 @@
       <c r="EJ8" t="inlineStr"/>
       <c r="EK8" t="inlineStr"/>
       <c r="EL8" t="inlineStr"/>
-      <c r="EM8" t="n">
-        <v>0.0003637871996033937</v>
-      </c>
+      <c r="EM8" t="inlineStr"/>
       <c r="EN8" t="n">
-        <v>0.4461042582988739</v>
+        <v>0.446</v>
       </c>
       <c r="EO8" t="n">
-        <v>0.0001622870188576963</v>
+        <v>0</v>
       </c>
       <c r="EP8" t="inlineStr"/>
       <c r="EQ8" t="inlineStr"/>
@@ -5552,22 +5390,22 @@
       <c r="FC8" t="inlineStr"/>
       <c r="FD8" t="inlineStr"/>
       <c r="FE8" t="n">
-        <v>0.001019495539367199</v>
+        <v>0.001</v>
       </c>
       <c r="FF8" t="n">
-        <v>0.5497950315475464</v>
+        <v>0.55</v>
       </c>
       <c r="FG8" t="n">
-        <v>0.000560513582228972</v>
+        <v>0.001</v>
       </c>
       <c r="FH8" t="n">
-        <v>0.726598858833313</v>
+        <v>0.727</v>
       </c>
       <c r="FI8" t="n">
-        <v>0.5548051595687866</v>
+        <v>0.555</v>
       </c>
       <c r="FJ8" t="n">
-        <v>0.4031207958175145</v>
+        <v>0.403</v>
       </c>
       <c r="FK8" t="inlineStr"/>
       <c r="FL8" t="inlineStr"/>
@@ -5575,14 +5413,12 @@
       <c r="FN8" t="inlineStr"/>
       <c r="FO8" t="inlineStr"/>
       <c r="FP8" t="inlineStr"/>
-      <c r="FQ8" t="n">
-        <v>0.000406003586249426</v>
-      </c>
+      <c r="FQ8" t="inlineStr"/>
       <c r="FR8" t="n">
-        <v>0.5567946434020996</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="FS8" t="n">
-        <v>0.0002260606220257227</v>
+        <v>0</v>
       </c>
       <c r="FT8" t="inlineStr"/>
       <c r="FU8" t="inlineStr"/>
@@ -5599,32 +5435,28 @@
       <c r="GF8" t="inlineStr"/>
       <c r="GG8" t="inlineStr"/>
       <c r="GH8" t="inlineStr"/>
-      <c r="GI8" t="n">
-        <v>0.0003705672279465944</v>
-      </c>
+      <c r="GI8" t="inlineStr"/>
       <c r="GJ8" t="n">
-        <v>0.4408858716487885</v>
+        <v>0.441</v>
       </c>
       <c r="GK8" t="n">
-        <v>0.0001633778552977095</v>
+        <v>0</v>
       </c>
       <c r="GL8" t="n">
-        <v>0.03856286033987999</v>
+        <v>0.039</v>
       </c>
       <c r="GM8" t="n">
-        <v>0.4610178470611572</v>
+        <v>0.461</v>
       </c>
       <c r="GN8" t="n">
-        <v>0.01777816685041156</v>
-      </c>
-      <c r="GO8" t="n">
-        <v>0.0003695043851621449</v>
-      </c>
+        <v>0.018</v>
+      </c>
+      <c r="GO8" t="inlineStr"/>
       <c r="GP8" t="n">
-        <v>0.4814366400241852</v>
+        <v>0.481</v>
       </c>
       <c r="GQ8" t="n">
-        <v>0.0001778929496666654</v>
+        <v>0</v>
       </c>
       <c r="GR8" t="inlineStr"/>
       <c r="GS8" t="inlineStr"/>
@@ -5632,53 +5464,43 @@
       <c r="GU8" t="inlineStr"/>
       <c r="GV8" t="inlineStr"/>
       <c r="GW8" t="inlineStr"/>
-      <c r="GX8" t="n">
-        <v>0.0003474180120974779</v>
-      </c>
+      <c r="GX8" t="inlineStr"/>
       <c r="GY8" t="n">
-        <v>0.5300662517547607</v>
+        <v>0.53</v>
       </c>
       <c r="GZ8" t="n">
-        <v>0.0001841545634646002</v>
-      </c>
-      <c r="HA8" t="n">
-        <v>0.0004102075181435794</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="HA8" t="inlineStr"/>
       <c r="HB8" t="n">
-        <v>0.4962268769741058</v>
+        <v>0.496</v>
       </c>
       <c r="HC8" t="n">
-        <v>0.0002035559956396872</v>
-      </c>
-      <c r="HD8" t="n">
-        <v>0.000410207110689953</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="HD8" t="inlineStr"/>
       <c r="HE8" t="n">
-        <v>0.4962269067764282</v>
+        <v>0.496</v>
       </c>
       <c r="HF8" t="n">
-        <v>0.0002035558056753713</v>
-      </c>
-      <c r="HG8" t="n">
-        <v>0.000410207110689953</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="HG8" t="inlineStr"/>
       <c r="HH8" t="n">
-        <v>0.4962269067764282</v>
+        <v>0.496</v>
       </c>
       <c r="HI8" t="n">
-        <v>0.0002035558056753713</v>
+        <v>0</v>
       </c>
       <c r="HJ8" t="inlineStr"/>
       <c r="HK8" t="inlineStr"/>
       <c r="HL8" t="inlineStr"/>
-      <c r="HM8" t="n">
-        <v>0.000352117873262614</v>
-      </c>
+      <c r="HM8" t="inlineStr"/>
       <c r="HN8" t="n">
-        <v>0.4280298948287964</v>
+        <v>0.428</v>
       </c>
       <c r="HO8" t="n">
-        <v>0.0001507169762599361</v>
+        <v>0</v>
       </c>
       <c r="HP8" t="inlineStr"/>
       <c r="HQ8" t="inlineStr"/>
@@ -5692,50 +5514,46 @@
       <c r="HY8" t="inlineStr"/>
       <c r="HZ8" t="inlineStr"/>
       <c r="IA8" t="inlineStr"/>
-      <c r="IB8" t="n">
-        <v>0.0003105879877693951</v>
-      </c>
+      <c r="IB8" t="inlineStr"/>
       <c r="IC8" t="n">
-        <v>0.309998095035553</v>
+        <v>0.31</v>
       </c>
       <c r="ID8" t="n">
-        <v>9.628168454943811e-05</v>
+        <v>0</v>
       </c>
       <c r="IE8" t="n">
-        <v>0.0006737752701155841</v>
+        <v>0.001</v>
       </c>
       <c r="IF8" t="n">
-        <v>0.5170761346817017</v>
+        <v>0.517</v>
       </c>
       <c r="IG8" t="n">
-        <v>0.0003483931123154857</v>
+        <v>0</v>
       </c>
       <c r="IH8" t="n">
-        <v>0.0006901848246343434</v>
+        <v>0.001</v>
       </c>
       <c r="II8" t="n">
-        <v>0.5038632750511169</v>
+        <v>0.504</v>
       </c>
       <c r="IJ8" t="n">
-        <v>0.0003477587861308411</v>
-      </c>
-      <c r="IK8" t="n">
-        <v>0.0003129032556898892</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="IK8" t="inlineStr"/>
       <c r="IL8" t="n">
-        <v>0.4999566674232483</v>
+        <v>0.5</v>
       </c>
       <c r="IM8" t="n">
-        <v>0.0001564380689406016</v>
+        <v>0</v>
       </c>
       <c r="IN8" t="n">
-        <v>0.6653873920440674</v>
+        <v>0.665</v>
       </c>
       <c r="IO8" t="n">
-        <v>0.4718460440635681</v>
+        <v>0.472</v>
       </c>
       <c r="IP8" t="n">
-        <v>0.3139604087057677</v>
+        <v>0.314</v>
       </c>
       <c r="IQ8" t="inlineStr"/>
       <c r="IR8" t="inlineStr"/>
@@ -5744,37 +5562,37 @@
       <c r="IU8" t="inlineStr"/>
       <c r="IV8" t="inlineStr"/>
       <c r="IW8" t="n">
-        <v>0.0005615924601443112</v>
+        <v>0.001</v>
       </c>
       <c r="IX8" t="n">
-        <v>0.4946322739124298</v>
+        <v>0.495</v>
       </c>
       <c r="IY8" t="n">
-        <v>0.0002777817555732563</v>
+        <v>0</v>
       </c>
       <c r="IZ8" t="inlineStr"/>
       <c r="JA8" t="inlineStr"/>
       <c r="JB8" t="inlineStr"/>
       <c r="JC8" t="n">
-        <v>0.0006762590492144227</v>
+        <v>0.001</v>
       </c>
       <c r="JD8" t="n">
-        <v>0.4789377748966217</v>
+        <v>0.479</v>
       </c>
       <c r="JE8" t="n">
-        <v>0.0003238860042844606</v>
+        <v>0</v>
       </c>
       <c r="JF8" t="inlineStr"/>
       <c r="JG8" t="inlineStr"/>
       <c r="JH8" t="inlineStr"/>
       <c r="JI8" t="n">
-        <v>0.0009168416145257652</v>
+        <v>0.001</v>
       </c>
       <c r="JJ8" t="n">
-        <v>0.502032458782196</v>
+        <v>0.502</v>
       </c>
       <c r="JK8" t="n">
-        <v>0.0004602842500542083</v>
+        <v>0</v>
       </c>
       <c r="JL8" t="inlineStr"/>
       <c r="JM8" t="inlineStr"/>
@@ -5785,32 +5603,28 @@
       <c r="JR8" t="inlineStr"/>
       <c r="JS8" t="inlineStr"/>
       <c r="JT8" t="inlineStr"/>
-      <c r="JU8" t="n">
-        <v>0.0004127658321522176</v>
-      </c>
+      <c r="JU8" t="inlineStr"/>
       <c r="JV8" t="n">
-        <v>0.5253615975379944</v>
+        <v>0.525</v>
       </c>
       <c r="JW8" t="n">
-        <v>0.0002168513169885887</v>
+        <v>0</v>
       </c>
       <c r="JX8" t="n">
-        <v>0.0009261633385904133</v>
+        <v>0.001</v>
       </c>
       <c r="JY8" t="n">
-        <v>0.5251535177230835</v>
+        <v>0.525</v>
       </c>
       <c r="JZ8" t="n">
-        <v>0.0004863779352469108</v>
-      </c>
-      <c r="KA8" t="n">
-        <v>0.0003226234694011509</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="KA8" t="inlineStr"/>
       <c r="KB8" t="n">
-        <v>0.4098951816558838</v>
+        <v>0.41</v>
       </c>
       <c r="KC8" t="n">
-        <v>0.0001322418055966362</v>
+        <v>0</v>
       </c>
       <c r="KD8" t="inlineStr"/>
       <c r="KE8" t="inlineStr"/>
@@ -5818,14 +5632,12 @@
       <c r="KG8" t="inlineStr"/>
       <c r="KH8" t="inlineStr"/>
       <c r="KI8" t="inlineStr"/>
-      <c r="KJ8" t="n">
-        <v>0.0003957873850595206</v>
-      </c>
+      <c r="KJ8" t="inlineStr"/>
       <c r="KK8" t="n">
-        <v>0.6610091924667358</v>
+        <v>0.661</v>
       </c>
       <c r="KL8" t="n">
-        <v>0.0002616190997867147</v>
+        <v>0</v>
       </c>
       <c r="KM8" t="inlineStr"/>
       <c r="KN8" t="inlineStr"/>
@@ -5848,14 +5660,12 @@
       <c r="LE8" t="inlineStr"/>
       <c r="LF8" t="inlineStr"/>
       <c r="LG8" t="inlineStr"/>
-      <c r="LH8" t="n">
-        <v>0.000340585014782846</v>
-      </c>
+      <c r="LH8" t="inlineStr"/>
       <c r="LI8" t="n">
-        <v>0.6885368824005127</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="LJ8" t="n">
-        <v>0.0002345053442709133</v>
+        <v>0</v>
       </c>
       <c r="LK8" t="inlineStr"/>
       <c r="LL8" t="inlineStr"/>
@@ -5892,13 +5702,13 @@
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="n">
-        <v>0.9706074595451355</v>
+        <v>0.971</v>
       </c>
       <c r="U9" t="n">
-        <v>0.3396194279193878</v>
+        <v>0.34</v>
       </c>
       <c r="V9" t="n">
-        <v>0.3296371501450093</v>
+        <v>0.33</v>
       </c>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
@@ -5910,13 +5720,13 @@
       <c r="AD9" t="inlineStr"/>
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="n">
-        <v>0.001093876897357404</v>
+        <v>0.001</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.3332393765449524</v>
+        <v>0.333</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.0003645228552923083</v>
+        <v>0</v>
       </c>
       <c r="AI9" t="inlineStr"/>
       <c r="AJ9" t="inlineStr"/>
@@ -5925,133 +5735,131 @@
       <c r="AM9" t="inlineStr"/>
       <c r="AN9" t="inlineStr"/>
       <c r="AO9" t="n">
-        <v>0.001462164334952831</v>
+        <v>0.001</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.3661949038505554</v>
+        <v>0.366</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.0005354371280517634</v>
+        <v>0.001</v>
       </c>
       <c r="AR9" t="n">
-        <v>0.05893751606345177</v>
+        <v>0.059</v>
       </c>
       <c r="AS9" t="n">
-        <v>0.3147044777870178</v>
+        <v>0.315</v>
       </c>
       <c r="AT9" t="n">
-        <v>0.01854790021481256</v>
+        <v>0.019</v>
       </c>
       <c r="AU9" t="n">
-        <v>0.877666175365448</v>
+        <v>0.878</v>
       </c>
       <c r="AV9" t="n">
-        <v>0.2910518050193787</v>
+        <v>0.291</v>
       </c>
       <c r="AW9" t="n">
-        <v>0.2554463245445682</v>
+        <v>0.255</v>
       </c>
       <c r="AX9" t="n">
-        <v>0.9692274332046509</v>
+        <v>0.969</v>
       </c>
       <c r="AY9" t="n">
-        <v>0.3323583900928497</v>
+        <v>0.332</v>
       </c>
       <c r="AZ9" t="n">
-        <v>0.3221308693337228</v>
-      </c>
-      <c r="BA9" t="n">
-        <v>0.0003125332877971232</v>
-      </c>
+        <v>0.322</v>
+      </c>
+      <c r="BA9" t="inlineStr"/>
       <c r="BB9" t="n">
-        <v>0.3427498638629913</v>
+        <v>0.343</v>
       </c>
       <c r="BC9" t="n">
-        <v>0.0001071207418451171</v>
+        <v>0</v>
       </c>
       <c r="BD9" t="inlineStr"/>
       <c r="BE9" t="inlineStr"/>
       <c r="BF9" t="inlineStr"/>
       <c r="BG9" t="n">
-        <v>0.009025638923048973</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="BH9" t="n">
-        <v>0.3145098686218262</v>
+        <v>0.315</v>
       </c>
       <c r="BI9" t="n">
-        <v>0.002838652511916173</v>
+        <v>0.003</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.670654833316803</v>
+        <v>0.671</v>
       </c>
       <c r="BK9" t="n">
-        <v>0.2900726497173309</v>
+        <v>0.29</v>
       </c>
       <c r="BL9" t="n">
-        <v>0.19453862454594</v>
+        <v>0.195</v>
       </c>
       <c r="BM9" t="n">
-        <v>0.5152230858802795</v>
+        <v>0.515</v>
       </c>
       <c r="BN9" t="n">
-        <v>0.2896857857704163</v>
+        <v>0.29</v>
       </c>
       <c r="BO9" t="n">
-        <v>0.1492528044802874</v>
+        <v>0.149</v>
       </c>
       <c r="BP9" t="n">
-        <v>0.9594396352767944</v>
+        <v>0.959</v>
       </c>
       <c r="BQ9" t="n">
-        <v>0.3308878242969513</v>
+        <v>0.331</v>
       </c>
       <c r="BR9" t="n">
-        <v>0.317466893460999</v>
+        <v>0.317</v>
       </c>
       <c r="BS9" t="n">
-        <v>0.003908931743353605</v>
+        <v>0.004</v>
       </c>
       <c r="BT9" t="n">
-        <v>0.3198983669281006</v>
+        <v>0.32</v>
       </c>
       <c r="BU9" t="n">
-        <v>0.001250460881132232</v>
+        <v>0.001</v>
       </c>
       <c r="BV9" t="n">
-        <v>0.00681459903717041</v>
+        <v>0.007</v>
       </c>
       <c r="BW9" t="n">
-        <v>0.3402609825134277</v>
+        <v>0.34</v>
       </c>
       <c r="BX9" t="n">
-        <v>0.002318742163822662</v>
+        <v>0.002</v>
       </c>
       <c r="BY9" t="n">
-        <v>0.9217461347579956</v>
+        <v>0.922</v>
       </c>
       <c r="BZ9" t="n">
-        <v>0.3384174108505249</v>
+        <v>0.338</v>
       </c>
       <c r="CA9" t="n">
-        <v>0.3119349403862799</v>
+        <v>0.312</v>
       </c>
       <c r="CB9" t="n">
-        <v>0.007812162861227989</v>
+        <v>0.008</v>
       </c>
       <c r="CC9" t="n">
-        <v>0.3326452970504761</v>
+        <v>0.333</v>
       </c>
       <c r="CD9" t="n">
-        <v>0.002598679235579882</v>
+        <v>0.003</v>
       </c>
       <c r="CE9" t="n">
-        <v>0.002401168923825026</v>
+        <v>0.002</v>
       </c>
       <c r="CF9" t="n">
-        <v>0.339859277009964</v>
+        <v>0.34</v>
       </c>
       <c r="CG9" t="n">
-        <v>0.0008160595344299665</v>
+        <v>0.001</v>
       </c>
       <c r="CH9" t="inlineStr"/>
       <c r="CI9" t="inlineStr"/>
@@ -6059,23 +5867,19 @@
       <c r="CK9" t="inlineStr"/>
       <c r="CL9" t="inlineStr"/>
       <c r="CM9" t="inlineStr"/>
-      <c r="CN9" t="n">
-        <v>0.0003504175401758403</v>
-      </c>
+      <c r="CN9" t="inlineStr"/>
       <c r="CO9" t="n">
-        <v>0.2903942465782166</v>
+        <v>0.29</v>
       </c>
       <c r="CP9" t="n">
-        <v>0.0001017592375671551</v>
-      </c>
-      <c r="CQ9" t="n">
-        <v>0.0003387499018572271</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="CQ9" t="inlineStr"/>
       <c r="CR9" t="n">
-        <v>0.2900564968585968</v>
+        <v>0.29</v>
       </c>
       <c r="CS9" t="n">
-        <v>9.825660984390076e-05</v>
+        <v>0</v>
       </c>
       <c r="CT9" t="inlineStr"/>
       <c r="CU9" t="inlineStr"/>
@@ -6095,14 +5899,12 @@
       <c r="DI9" t="inlineStr"/>
       <c r="DJ9" t="inlineStr"/>
       <c r="DK9" t="inlineStr"/>
-      <c r="DL9" t="n">
-        <v>0.0002473825879860669</v>
-      </c>
+      <c r="DL9" t="inlineStr"/>
       <c r="DM9" t="n">
-        <v>0.3339318633079529</v>
+        <v>0.334</v>
       </c>
       <c r="DN9" t="n">
-        <v>8.260892855613093e-05</v>
+        <v>0</v>
       </c>
       <c r="DO9" t="inlineStr"/>
       <c r="DP9" t="inlineStr"/>
@@ -6120,25 +5922,23 @@
       <c r="EB9" t="inlineStr"/>
       <c r="EC9" t="inlineStr"/>
       <c r="ED9" t="n">
-        <v>0.0009309566812589765</v>
+        <v>0.001</v>
       </c>
       <c r="EE9" t="n">
-        <v>0.3301744759082794</v>
+        <v>0.33</v>
       </c>
       <c r="EF9" t="n">
-        <v>0.0003073781343279937</v>
+        <v>0</v>
       </c>
       <c r="EG9" t="inlineStr"/>
       <c r="EH9" t="inlineStr"/>
       <c r="EI9" t="inlineStr"/>
-      <c r="EJ9" t="n">
-        <v>0.0002693291462492198</v>
-      </c>
+      <c r="EJ9" t="inlineStr"/>
       <c r="EK9" t="n">
-        <v>0.3331267237663269</v>
+        <v>0.333</v>
       </c>
       <c r="EL9" t="n">
-        <v>8.97207361047845e-05</v>
+        <v>0</v>
       </c>
       <c r="EM9" t="inlineStr"/>
       <c r="EN9" t="inlineStr"/>
@@ -6152,14 +5952,12 @@
       <c r="EV9" t="inlineStr"/>
       <c r="EW9" t="inlineStr"/>
       <c r="EX9" t="inlineStr"/>
-      <c r="EY9" t="n">
-        <v>0.0004091972950845957</v>
-      </c>
+      <c r="EY9" t="inlineStr"/>
       <c r="EZ9" t="n">
-        <v>0.3150666356086731</v>
+        <v>0.315</v>
       </c>
       <c r="FA9" t="n">
-        <v>0.000128924415062473</v>
+        <v>0</v>
       </c>
       <c r="FB9" t="inlineStr"/>
       <c r="FC9" t="inlineStr"/>
@@ -6171,13 +5969,13 @@
       <c r="FI9" t="inlineStr"/>
       <c r="FJ9" t="inlineStr"/>
       <c r="FK9" t="n">
-        <v>0.1185019090771675</v>
+        <v>0.119</v>
       </c>
       <c r="FL9" t="n">
-        <v>0.3327697515487671</v>
+        <v>0.333</v>
       </c>
       <c r="FM9" t="n">
-        <v>0.03943385084166362</v>
+        <v>0.039</v>
       </c>
       <c r="FN9" t="inlineStr"/>
       <c r="FO9" t="inlineStr"/>
@@ -6186,13 +5984,13 @@
       <c r="FR9" t="inlineStr"/>
       <c r="FS9" t="inlineStr"/>
       <c r="FT9" t="n">
-        <v>0.5935564041137695</v>
+        <v>0.594</v>
       </c>
       <c r="FU9" t="n">
-        <v>0.3403068780899048</v>
+        <v>0.34</v>
       </c>
       <c r="FV9" t="n">
-        <v>0.2019913268542268</v>
+        <v>0.202</v>
       </c>
       <c r="FW9" t="inlineStr"/>
       <c r="FX9" t="inlineStr"/>
@@ -6200,23 +5998,19 @@
       <c r="FZ9" t="inlineStr"/>
       <c r="GA9" t="inlineStr"/>
       <c r="GB9" t="inlineStr"/>
-      <c r="GC9" t="n">
-        <v>0.0004253729712218046</v>
-      </c>
+      <c r="GC9" t="inlineStr"/>
       <c r="GD9" t="n">
-        <v>0.3405442833900452</v>
+        <v>0.341</v>
       </c>
       <c r="GE9" t="n">
-        <v>0.0001448583336582238</v>
-      </c>
-      <c r="GF9" t="n">
-        <v>0.0003139790205750614</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="GF9" t="inlineStr"/>
       <c r="GG9" t="n">
-        <v>0.3370152115821838</v>
+        <v>0.337</v>
       </c>
       <c r="GH9" t="n">
-        <v>0.0001058157060514712</v>
+        <v>0</v>
       </c>
       <c r="GI9" t="inlineStr"/>
       <c r="GJ9" t="inlineStr"/>
@@ -6228,22 +6022,20 @@
       <c r="GP9" t="inlineStr"/>
       <c r="GQ9" t="inlineStr"/>
       <c r="GR9" t="n">
-        <v>0.001086655305698514</v>
+        <v>0.001</v>
       </c>
       <c r="GS9" t="n">
-        <v>0.3328761160373688</v>
+        <v>0.333</v>
       </c>
       <c r="GT9" t="n">
-        <v>0.000361721597632321</v>
-      </c>
-      <c r="GU9" t="n">
-        <v>0.000312501098960638</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="GU9" t="inlineStr"/>
       <c r="GV9" t="n">
-        <v>0.3273706138134003</v>
+        <v>0.327</v>
       </c>
       <c r="GW9" t="n">
-        <v>0.0001023036765841062</v>
+        <v>0</v>
       </c>
       <c r="GX9" t="inlineStr"/>
       <c r="GY9" t="inlineStr"/>
@@ -6258,25 +6050,23 @@
       <c r="HH9" t="inlineStr"/>
       <c r="HI9" t="inlineStr"/>
       <c r="HJ9" t="n">
-        <v>0.0005665670032612979</v>
+        <v>0.001</v>
       </c>
       <c r="HK9" t="n">
-        <v>0.3451867997646332</v>
+        <v>0.345</v>
       </c>
       <c r="HL9" t="n">
-        <v>0.0001955714507080059</v>
+        <v>0</v>
       </c>
       <c r="HM9" t="inlineStr"/>
       <c r="HN9" t="inlineStr"/>
       <c r="HO9" t="inlineStr"/>
-      <c r="HP9" t="n">
-        <v>0.0003124730719719082</v>
-      </c>
+      <c r="HP9" t="inlineStr"/>
       <c r="HQ9" t="n">
-        <v>0.3336398601531982</v>
+        <v>0.334</v>
       </c>
       <c r="HR9" t="n">
-        <v>0.0001042534720343477</v>
+        <v>0</v>
       </c>
       <c r="HS9" t="inlineStr"/>
       <c r="HT9" t="inlineStr"/>
@@ -6317,26 +6107,24 @@
       <c r="JC9" t="inlineStr"/>
       <c r="JD9" t="inlineStr"/>
       <c r="JE9" t="inlineStr"/>
-      <c r="JF9" t="n">
-        <v>0.0003200739156454802</v>
-      </c>
+      <c r="JF9" t="inlineStr"/>
       <c r="JG9" t="n">
-        <v>0.340257465839386</v>
+        <v>0.34</v>
       </c>
       <c r="JH9" t="n">
-        <v>0.0001089075394188205</v>
+        <v>0</v>
       </c>
       <c r="JI9" t="inlineStr"/>
       <c r="JJ9" t="inlineStr"/>
       <c r="JK9" t="inlineStr"/>
       <c r="JL9" t="n">
-        <v>0.0006588773103430867</v>
+        <v>0.001</v>
       </c>
       <c r="JM9" t="n">
-        <v>0.3466519117355347</v>
+        <v>0.347</v>
       </c>
       <c r="JN9" t="n">
-        <v>0.0002284010792295982</v>
+        <v>0</v>
       </c>
       <c r="JO9" t="inlineStr"/>
       <c r="JP9" t="inlineStr"/>
@@ -6356,14 +6144,12 @@
       <c r="KD9" t="inlineStr"/>
       <c r="KE9" t="inlineStr"/>
       <c r="KF9" t="inlineStr"/>
-      <c r="KG9" t="n">
-        <v>0.0003833376395050436</v>
-      </c>
+      <c r="KG9" t="inlineStr"/>
       <c r="KH9" t="n">
-        <v>0.3347676396369934</v>
+        <v>0.335</v>
       </c>
       <c r="KI9" t="n">
-        <v>0.0001283290367611201</v>
+        <v>0</v>
       </c>
       <c r="KJ9" t="inlineStr"/>
       <c r="KK9" t="inlineStr"/>
@@ -6381,13 +6167,13 @@
       <c r="KW9" t="inlineStr"/>
       <c r="KX9" t="inlineStr"/>
       <c r="KY9" t="n">
-        <v>0.0008177368436008692</v>
+        <v>0.001</v>
       </c>
       <c r="KZ9" t="n">
-        <v>0.3397031128406525</v>
+        <v>0.34</v>
       </c>
       <c r="LA9" t="n">
-        <v>0.000277787751255705</v>
+        <v>0</v>
       </c>
       <c r="LB9" t="inlineStr"/>
       <c r="LC9" t="inlineStr"/>
@@ -6430,25 +6216,25 @@
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="n">
-        <v>0.002255158964544535</v>
+        <v>0.002</v>
       </c>
       <c r="R10" t="n">
-        <v>0.0562230609357357</v>
+        <v>0.056</v>
       </c>
       <c r="S10" t="n">
-        <v>0.000126791939883358</v>
+        <v>0</v>
       </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="n">
-        <v>0.002244990319013596</v>
+        <v>0.002</v>
       </c>
       <c r="X10" t="n">
-        <v>0.08278480172157288</v>
+        <v>0.083</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.0001858510784263911</v>
+        <v>0</v>
       </c>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
@@ -6481,13 +6267,13 @@
       <c r="BB10" t="inlineStr"/>
       <c r="BC10" t="inlineStr"/>
       <c r="BD10" t="n">
-        <v>0.002499517751857638</v>
+        <v>0.002</v>
       </c>
       <c r="BE10" t="n">
-        <v>0.1252408623695374</v>
+        <v>0.125</v>
       </c>
       <c r="BF10" t="n">
-        <v>0.0003130417587506179</v>
+        <v>0</v>
       </c>
       <c r="BG10" t="inlineStr"/>
       <c r="BH10" t="inlineStr"/>
@@ -6529,13 +6315,13 @@
       <c r="CR10" t="inlineStr"/>
       <c r="CS10" t="inlineStr"/>
       <c r="CT10" t="n">
-        <v>0.298565000295639</v>
+        <v>0.299</v>
       </c>
       <c r="CU10" t="n">
-        <v>0.2716094851493835</v>
+        <v>0.272</v>
       </c>
       <c r="CV10" t="n">
-        <v>0.08109308601392407</v>
+        <v>0.081</v>
       </c>
       <c r="CW10" t="inlineStr"/>
       <c r="CX10" t="inlineStr"/>
@@ -6550,13 +6336,13 @@
       <c r="DG10" t="inlineStr"/>
       <c r="DH10" t="inlineStr"/>
       <c r="DI10" t="n">
-        <v>0.2066100239753723</v>
+        <v>0.207</v>
       </c>
       <c r="DJ10" t="n">
-        <v>0.2946513891220093</v>
+        <v>0.295</v>
       </c>
       <c r="DK10" t="n">
-        <v>0.06087793057087509</v>
+        <v>0.061</v>
       </c>
       <c r="DL10" t="inlineStr"/>
       <c r="DM10" t="inlineStr"/>
@@ -6580,13 +6366,13 @@
       <c r="EE10" t="inlineStr"/>
       <c r="EF10" t="inlineStr"/>
       <c r="EG10" t="n">
-        <v>0.3903506100177765</v>
+        <v>0.39</v>
       </c>
       <c r="EH10" t="n">
-        <v>0.3521092534065247</v>
+        <v>0.352</v>
       </c>
       <c r="EI10" t="n">
-        <v>0.1374460618601407</v>
+        <v>0.137</v>
       </c>
       <c r="EJ10" t="inlineStr"/>
       <c r="EK10" t="inlineStr"/>
@@ -6601,25 +6387,25 @@
       <c r="ET10" t="inlineStr"/>
       <c r="EU10" t="inlineStr"/>
       <c r="EV10" t="n">
-        <v>0.3265285491943359</v>
+        <v>0.327</v>
       </c>
       <c r="EW10" t="n">
-        <v>0.1948638111352921</v>
+        <v>0.195</v>
       </c>
       <c r="EX10" t="n">
-        <v>0.063628597540486</v>
+        <v>0.064</v>
       </c>
       <c r="EY10" t="inlineStr"/>
       <c r="EZ10" t="inlineStr"/>
       <c r="FA10" t="inlineStr"/>
       <c r="FB10" t="n">
-        <v>0.198619157075882</v>
+        <v>0.199</v>
       </c>
       <c r="FC10" t="n">
-        <v>0.2295186817646027</v>
+        <v>0.23</v>
       </c>
       <c r="FD10" t="n">
-        <v>0.04558680710525298</v>
+        <v>0.046</v>
       </c>
       <c r="FE10" t="inlineStr"/>
       <c r="FF10" t="inlineStr"/>
@@ -6643,13 +6429,13 @@
       <c r="FX10" t="inlineStr"/>
       <c r="FY10" t="inlineStr"/>
       <c r="FZ10" t="n">
-        <v>0.5888562202453613</v>
+        <v>0.589</v>
       </c>
       <c r="GA10" t="n">
-        <v>0.3315315544605255</v>
+        <v>0.332</v>
       </c>
       <c r="GB10" t="n">
-        <v>0.1952244180516942</v>
+        <v>0.195</v>
       </c>
       <c r="GC10" t="inlineStr"/>
       <c r="GD10" t="inlineStr"/>
@@ -6697,22 +6483,22 @@
       <c r="HT10" t="inlineStr"/>
       <c r="HU10" t="inlineStr"/>
       <c r="HV10" t="n">
-        <v>0.2774701118469238</v>
+        <v>0.277</v>
       </c>
       <c r="HW10" t="n">
-        <v>0.3653570413589478</v>
+        <v>0.365</v>
       </c>
       <c r="HX10" t="n">
-        <v>0.1013756591299284</v>
+        <v>0.101</v>
       </c>
       <c r="HY10" t="n">
-        <v>0.2805783748626709</v>
+        <v>0.281</v>
       </c>
       <c r="HZ10" t="n">
-        <v>0.3373971879482269</v>
+        <v>0.337</v>
       </c>
       <c r="IA10" t="n">
-        <v>0.09466635467774864</v>
+        <v>0.095</v>
       </c>
       <c r="IB10" t="inlineStr"/>
       <c r="IC10" t="inlineStr"/>
@@ -6730,34 +6516,34 @@
       <c r="IO10" t="inlineStr"/>
       <c r="IP10" t="inlineStr"/>
       <c r="IQ10" t="n">
-        <v>0.2539681196212769</v>
+        <v>0.254</v>
       </c>
       <c r="IR10" t="n">
-        <v>0.347613662481308</v>
+        <v>0.348</v>
       </c>
       <c r="IS10" t="n">
-        <v>0.08828278821504298</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="IT10" t="n">
-        <v>0.2370169162750244</v>
+        <v>0.237</v>
       </c>
       <c r="IU10" t="n">
-        <v>0.3052501082420349</v>
+        <v>0.305</v>
       </c>
       <c r="IV10" t="n">
-        <v>0.07234943934814453</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="IW10" t="inlineStr"/>
       <c r="IX10" t="inlineStr"/>
       <c r="IY10" t="inlineStr"/>
       <c r="IZ10" t="n">
-        <v>0.2379149794578552</v>
+        <v>0.238</v>
       </c>
       <c r="JA10" t="n">
-        <v>0.3087382018566132</v>
+        <v>0.309</v>
       </c>
       <c r="JB10" t="n">
-        <v>0.07345344295257128</v>
+        <v>0.073</v>
       </c>
       <c r="JC10" t="inlineStr"/>
       <c r="JD10" t="inlineStr"/>
@@ -6787,13 +6573,13 @@
       <c r="KB10" t="inlineStr"/>
       <c r="KC10" t="inlineStr"/>
       <c r="KD10" t="n">
-        <v>0.4110191464424133</v>
+        <v>0.411</v>
       </c>
       <c r="KE10" t="n">
-        <v>0.2880536615848541</v>
+        <v>0.288</v>
       </c>
       <c r="KF10" t="n">
-        <v>0.1183955701142185</v>
+        <v>0.118</v>
       </c>
       <c r="KG10" t="inlineStr"/>
       <c r="KH10" t="inlineStr"/>
@@ -6820,13 +6606,13 @@
       <c r="LC10" t="inlineStr"/>
       <c r="LD10" t="inlineStr"/>
       <c r="LE10" t="n">
-        <v>0.2955038249492645</v>
+        <v>0.296</v>
       </c>
       <c r="LF10" t="n">
-        <v>0.4307330548763275</v>
+        <v>0.431</v>
       </c>
       <c r="LG10" t="n">
-        <v>0.1272832652480362</v>
+        <v>0.127</v>
       </c>
       <c r="LH10" t="inlineStr"/>
       <c r="LI10" t="inlineStr"/>
@@ -6838,13 +6624,13 @@
       <c r="LO10" t="inlineStr"/>
       <c r="LP10" t="inlineStr"/>
       <c r="LQ10" t="n">
-        <v>0.2192463427782059</v>
+        <v>0.219</v>
       </c>
       <c r="LR10" t="n">
-        <v>0.3174873292446136</v>
+        <v>0.317</v>
       </c>
       <c r="LS10" t="n">
-        <v>0.06960793581530167</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -6869,25 +6655,25 @@
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="n">
-        <v>0.9950023293495178</v>
+        <v>0.995</v>
       </c>
       <c r="R11" t="n">
-        <v>0.3942170143127441</v>
+        <v>0.394</v>
       </c>
       <c r="S11" t="n">
-        <v>0.3922468475103926</v>
+        <v>0.392</v>
       </c>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="n">
-        <v>0.7712607979774475</v>
+        <v>0.771</v>
       </c>
       <c r="X11" t="n">
-        <v>0.153375968337059</v>
+        <v>0.153</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.1182928717302039</v>
+        <v>0.118</v>
       </c>
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="inlineStr"/>
@@ -6920,13 +6706,13 @@
       <c r="BB11" t="inlineStr"/>
       <c r="BC11" t="inlineStr"/>
       <c r="BD11" t="n">
-        <v>0.9695455431938171</v>
+        <v>0.97</v>
       </c>
       <c r="BE11" t="n">
-        <v>0.1706218719482422</v>
+        <v>0.171</v>
       </c>
       <c r="BF11" t="n">
-        <v>0.1654256755188044</v>
+        <v>0.165</v>
       </c>
       <c r="BG11" t="inlineStr"/>
       <c r="BH11" t="inlineStr"/>
@@ -6968,13 +6754,13 @@
       <c r="CR11" t="inlineStr"/>
       <c r="CS11" t="inlineStr"/>
       <c r="CT11" t="n">
-        <v>0.0006525885546579957</v>
+        <v>0.001</v>
       </c>
       <c r="CU11" t="n">
-        <v>0.04998964443802834</v>
+        <v>0.05</v>
       </c>
       <c r="CV11" t="n">
-        <v>3.262266981168003e-05</v>
+        <v>0</v>
       </c>
       <c r="CW11" t="inlineStr"/>
       <c r="CX11" t="inlineStr"/>
@@ -6988,14 +6774,12 @@
       <c r="DF11" t="inlineStr"/>
       <c r="DG11" t="inlineStr"/>
       <c r="DH11" t="inlineStr"/>
-      <c r="DI11" t="n">
-        <v>0.0002236352302134037</v>
-      </c>
+      <c r="DI11" t="inlineStr"/>
       <c r="DJ11" t="n">
-        <v>0.1881195902824402</v>
+        <v>0.188</v>
       </c>
       <c r="DK11" t="n">
-        <v>4.207016788046469e-05</v>
+        <v>0</v>
       </c>
       <c r="DL11" t="inlineStr"/>
       <c r="DM11" t="inlineStr"/>
@@ -7019,13 +6803,13 @@
       <c r="EE11" t="inlineStr"/>
       <c r="EF11" t="inlineStr"/>
       <c r="EG11" t="n">
-        <v>0.002366490894928575</v>
+        <v>0.002</v>
       </c>
       <c r="EH11" t="n">
-        <v>0.06116156280040741</v>
+        <v>0.061</v>
       </c>
       <c r="EI11" t="n">
-        <v>0.0001447382814867663</v>
+        <v>0</v>
       </c>
       <c r="EJ11" t="inlineStr"/>
       <c r="EK11" t="inlineStr"/>
@@ -7039,26 +6823,24 @@
       <c r="ES11" t="inlineStr"/>
       <c r="ET11" t="inlineStr"/>
       <c r="EU11" t="inlineStr"/>
-      <c r="EV11" t="n">
-        <v>0.0002124151214957237</v>
-      </c>
+      <c r="EV11" t="inlineStr"/>
       <c r="EW11" t="n">
-        <v>0.2129285335540771</v>
+        <v>0.213</v>
       </c>
       <c r="EX11" t="n">
-        <v>4.522924032479558e-05</v>
+        <v>0</v>
       </c>
       <c r="EY11" t="inlineStr"/>
       <c r="EZ11" t="inlineStr"/>
       <c r="FA11" t="inlineStr"/>
       <c r="FB11" t="n">
-        <v>0.0006468875799328089</v>
+        <v>0.001</v>
       </c>
       <c r="FC11" t="n">
-        <v>0.3289362192153931</v>
+        <v>0.329</v>
       </c>
       <c r="FD11" t="n">
-        <v>0.0002127847548004935</v>
+        <v>0</v>
       </c>
       <c r="FE11" t="inlineStr"/>
       <c r="FF11" t="inlineStr"/>
@@ -7081,14 +6863,12 @@
       <c r="FW11" t="inlineStr"/>
       <c r="FX11" t="inlineStr"/>
       <c r="FY11" t="inlineStr"/>
-      <c r="FZ11" t="n">
-        <v>0.0003865206090267748</v>
-      </c>
+      <c r="FZ11" t="inlineStr"/>
       <c r="GA11" t="n">
-        <v>0.19254170358181</v>
+        <v>0.193</v>
       </c>
       <c r="GB11" t="n">
-        <v>7.442133653149394e-05</v>
+        <v>0</v>
       </c>
       <c r="GC11" t="inlineStr"/>
       <c r="GD11" t="inlineStr"/>
@@ -7135,23 +6915,19 @@
       <c r="HS11" t="inlineStr"/>
       <c r="HT11" t="inlineStr"/>
       <c r="HU11" t="inlineStr"/>
-      <c r="HV11" t="n">
-        <v>0.0004358862643130124</v>
-      </c>
+      <c r="HV11" t="inlineStr"/>
       <c r="HW11" t="n">
-        <v>0.1664101034402847</v>
+        <v>0.166</v>
       </c>
       <c r="HX11" t="n">
-        <v>7.253587833252768e-05</v>
-      </c>
-      <c r="HY11" t="n">
-        <v>0.000180597256985493</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="HY11" t="inlineStr"/>
       <c r="HZ11" t="n">
-        <v>0.1349434852600098</v>
+        <v>0.135</v>
       </c>
       <c r="IA11" t="n">
-        <v>2.437042328602007e-05</v>
+        <v>0</v>
       </c>
       <c r="IB11" t="inlineStr"/>
       <c r="IC11" t="inlineStr"/>
@@ -7168,35 +6944,33 @@
       <c r="IN11" t="inlineStr"/>
       <c r="IO11" t="inlineStr"/>
       <c r="IP11" t="inlineStr"/>
-      <c r="IQ11" t="n">
-        <v>0.0001590020838193595</v>
-      </c>
+      <c r="IQ11" t="inlineStr"/>
       <c r="IR11" t="n">
-        <v>0.1026419177651405</v>
+        <v>0.103</v>
       </c>
       <c r="IS11" t="n">
-        <v>1.632027881187268e-05</v>
+        <v>0</v>
       </c>
       <c r="IT11" t="n">
-        <v>0.0009577865130268037</v>
+        <v>0.001</v>
       </c>
       <c r="IU11" t="n">
-        <v>0.1452485769987106</v>
+        <v>0.145</v>
       </c>
       <c r="IV11" t="n">
-        <v>0.0001391171280857003</v>
+        <v>0</v>
       </c>
       <c r="IW11" t="inlineStr"/>
       <c r="IX11" t="inlineStr"/>
       <c r="IY11" t="inlineStr"/>
       <c r="IZ11" t="n">
-        <v>0.001225997693836689</v>
+        <v>0.001</v>
       </c>
       <c r="JA11" t="n">
-        <v>0.135805755853653</v>
+        <v>0.136</v>
       </c>
       <c r="JB11" t="n">
-        <v>0.0001664975434863269</v>
+        <v>0</v>
       </c>
       <c r="JC11" t="inlineStr"/>
       <c r="JD11" t="inlineStr"/>
@@ -7226,13 +7000,13 @@
       <c r="KB11" t="inlineStr"/>
       <c r="KC11" t="inlineStr"/>
       <c r="KD11" t="n">
-        <v>0.7484806180000305</v>
+        <v>0.748</v>
       </c>
       <c r="KE11" t="n">
-        <v>0.2019944041967392</v>
+        <v>0.202</v>
       </c>
       <c r="KF11" t="n">
-        <v>0.1511888964857233</v>
+        <v>0.151</v>
       </c>
       <c r="KG11" t="inlineStr"/>
       <c r="KH11" t="inlineStr"/>
@@ -7259,13 +7033,13 @@
       <c r="LC11" t="inlineStr"/>
       <c r="LD11" t="inlineStr"/>
       <c r="LE11" t="n">
-        <v>0.0006723166443407536</v>
+        <v>0.001</v>
       </c>
       <c r="LF11" t="n">
-        <v>0.09827776998281479</v>
+        <v>0.098</v>
       </c>
       <c r="LG11" t="n">
-        <v>6.607378052813848e-05</v>
+        <v>0</v>
       </c>
       <c r="LH11" t="inlineStr"/>
       <c r="LI11" t="inlineStr"/>
@@ -7276,14 +7050,12 @@
       <c r="LN11" t="inlineStr"/>
       <c r="LO11" t="inlineStr"/>
       <c r="LP11" t="inlineStr"/>
-      <c r="LQ11" t="n">
-        <v>0.0001760323502821848</v>
-      </c>
+      <c r="LQ11" t="inlineStr"/>
       <c r="LR11" t="n">
-        <v>0.1359386146068573</v>
+        <v>0.136</v>
       </c>
       <c r="LS11" t="n">
-        <v>2.392959382334922e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -7296,34 +7068,30 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.002512543462216854</v>
+        <v>0.003</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5462933778762817</v>
+        <v>0.546</v>
       </c>
       <c r="G12" t="n">
-        <v>0.001372585855035413</v>
+        <v>0.001</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="n">
-        <v>8.425604028161615e-05</v>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="n">
-        <v>0.5173661112785339</v>
+        <v>0.517</v>
       </c>
       <c r="M12" t="n">
-        <v>4.359121991222726e-05</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.000126361264847219</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>0.5038175582885742</v>
+        <v>0.504</v>
       </c>
       <c r="P12" t="n">
-        <v>6.366302391758172e-05</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
@@ -7344,13 +7112,13 @@
       <c r="AG12" t="inlineStr"/>
       <c r="AH12" t="inlineStr"/>
       <c r="AI12" t="n">
-        <v>0.003594587789848447</v>
+        <v>0.004</v>
       </c>
       <c r="AJ12" t="n">
-        <v>0.499147891998291</v>
+        <v>0.499</v>
       </c>
       <c r="AK12" t="n">
-        <v>0.001794230917905648</v>
+        <v>0.002</v>
       </c>
       <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="inlineStr"/>
@@ -7415,14 +7183,12 @@
       <c r="CT12" t="inlineStr"/>
       <c r="CU12" t="inlineStr"/>
       <c r="CV12" t="inlineStr"/>
-      <c r="CW12" t="n">
-        <v>6.243226380320266e-05</v>
-      </c>
+      <c r="CW12" t="inlineStr"/>
       <c r="CX12" t="n">
-        <v>0.5653545260429382</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="CY12" t="n">
-        <v>3.529636291224733e-05</v>
+        <v>0</v>
       </c>
       <c r="CZ12" t="inlineStr"/>
       <c r="DA12" t="inlineStr"/>
@@ -7442,41 +7208,33 @@
       <c r="DO12" t="inlineStr"/>
       <c r="DP12" t="inlineStr"/>
       <c r="DQ12" t="inlineStr"/>
-      <c r="DR12" t="n">
-        <v>0.0002283357025589794</v>
-      </c>
+      <c r="DR12" t="inlineStr"/>
       <c r="DS12" t="n">
-        <v>0.5450702309608459</v>
+        <v>0.545</v>
       </c>
       <c r="DT12" t="n">
-        <v>0.0001244589941304299</v>
-      </c>
-      <c r="DU12" t="n">
-        <v>5.554901508730836e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="DU12" t="inlineStr"/>
       <c r="DV12" t="n">
-        <v>0.5274627804756165</v>
+        <v>0.527</v>
       </c>
       <c r="DW12" t="n">
-        <v>2.930003795063364e-05</v>
-      </c>
-      <c r="DX12" t="n">
-        <v>7.865405495977029e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="DX12" t="inlineStr"/>
       <c r="DY12" t="n">
-        <v>0.6389243006706238</v>
+        <v>0.639</v>
       </c>
       <c r="DZ12" t="n">
-        <v>5.025398706008004e-05</v>
-      </c>
-      <c r="EA12" t="n">
-        <v>6.264235707931221e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="EA12" t="inlineStr"/>
       <c r="EB12" t="n">
-        <v>0.4255427420139313</v>
+        <v>0.426</v>
       </c>
       <c r="EC12" t="n">
-        <v>2.665700039774632e-05</v>
+        <v>0</v>
       </c>
       <c r="ED12" t="inlineStr"/>
       <c r="EE12" t="inlineStr"/>
@@ -7490,23 +7248,19 @@
       <c r="EM12" t="inlineStr"/>
       <c r="EN12" t="inlineStr"/>
       <c r="EO12" t="inlineStr"/>
-      <c r="EP12" t="n">
-        <v>0.000146601174492389</v>
-      </c>
+      <c r="EP12" t="inlineStr"/>
       <c r="EQ12" t="n">
-        <v>0.4796972274780273</v>
+        <v>0.48</v>
       </c>
       <c r="ER12" t="n">
-        <v>7.032417694902149e-05</v>
-      </c>
-      <c r="ES12" t="n">
-        <v>6.502451287815347e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="ES12" t="inlineStr"/>
       <c r="ET12" t="n">
-        <v>0.7057353258132935</v>
+        <v>0.706</v>
       </c>
       <c r="EU12" t="n">
-        <v>4.589009578191434e-05</v>
+        <v>0</v>
       </c>
       <c r="EV12" t="inlineStr"/>
       <c r="EW12" t="inlineStr"/>
@@ -7526,14 +7280,12 @@
       <c r="FK12" t="inlineStr"/>
       <c r="FL12" t="inlineStr"/>
       <c r="FM12" t="inlineStr"/>
-      <c r="FN12" t="n">
-        <v>0.0003851279034279287</v>
-      </c>
+      <c r="FN12" t="inlineStr"/>
       <c r="FO12" t="n">
-        <v>0.6897847056388855</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="FP12" t="n">
-        <v>0.0002656553374993549</v>
+        <v>0</v>
       </c>
       <c r="FQ12" t="inlineStr"/>
       <c r="FR12" t="inlineStr"/>
@@ -7541,14 +7293,12 @@
       <c r="FT12" t="inlineStr"/>
       <c r="FU12" t="inlineStr"/>
       <c r="FV12" t="inlineStr"/>
-      <c r="FW12" t="n">
-        <v>5.3116847993806e-05</v>
-      </c>
+      <c r="FW12" t="inlineStr"/>
       <c r="FX12" t="n">
-        <v>0.5975146293640137</v>
+        <v>0.598</v>
       </c>
       <c r="FY12" t="n">
-        <v>3.173809374200365e-05</v>
+        <v>0</v>
       </c>
       <c r="FZ12" t="inlineStr"/>
       <c r="GA12" t="inlineStr"/>
@@ -7595,14 +7345,12 @@
       <c r="HP12" t="inlineStr"/>
       <c r="HQ12" t="inlineStr"/>
       <c r="HR12" t="inlineStr"/>
-      <c r="HS12" t="n">
-        <v>0.0001805636711651459</v>
-      </c>
+      <c r="HS12" t="inlineStr"/>
       <c r="HT12" t="n">
-        <v>0.4717152416706085</v>
+        <v>0.472</v>
       </c>
       <c r="HU12" t="n">
-        <v>8.51746357805991e-05</v>
+        <v>0</v>
       </c>
       <c r="HV12" t="inlineStr"/>
       <c r="HW12" t="inlineStr"/>
@@ -7649,23 +7397,19 @@
       <c r="JL12" t="inlineStr"/>
       <c r="JM12" t="inlineStr"/>
       <c r="JN12" t="inlineStr"/>
-      <c r="JO12" t="n">
-        <v>5.239657548372634e-05</v>
-      </c>
+      <c r="JO12" t="inlineStr"/>
       <c r="JP12" t="n">
-        <v>0.2734697759151459</v>
+        <v>0.273</v>
       </c>
       <c r="JQ12" t="n">
-        <v>1.432887975625567e-05</v>
-      </c>
-      <c r="JR12" t="n">
-        <v>0.00020996255625505</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="JR12" t="inlineStr"/>
       <c r="JS12" t="n">
-        <v>0.3023075461387634</v>
+        <v>0.302</v>
       </c>
       <c r="JT12" t="n">
-        <v>6.347326516248624e-05</v>
+        <v>0</v>
       </c>
       <c r="JU12" t="inlineStr"/>
       <c r="JV12" t="inlineStr"/>
@@ -7685,53 +7429,43 @@
       <c r="KJ12" t="inlineStr"/>
       <c r="KK12" t="inlineStr"/>
       <c r="KL12" t="inlineStr"/>
-      <c r="KM12" t="n">
-        <v>5.1309685659362e-05</v>
-      </c>
+      <c r="KM12" t="inlineStr"/>
       <c r="KN12" t="n">
-        <v>0.3678361177444458</v>
+        <v>0.368</v>
       </c>
       <c r="KO12" t="n">
-        <v>1.887355557562758e-05</v>
-      </c>
-      <c r="KP12" t="n">
-        <v>5.113027873449028e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="KP12" t="inlineStr"/>
       <c r="KQ12" t="n">
-        <v>0.3857069909572601</v>
+        <v>0.386</v>
       </c>
       <c r="KR12" t="n">
-        <v>1.972130595748623e-05</v>
-      </c>
-      <c r="KS12" t="n">
-        <v>5.300436896504834e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="KS12" t="inlineStr"/>
       <c r="KT12" t="n">
-        <v>0.3577251136302948</v>
+        <v>0.358</v>
       </c>
       <c r="KU12" t="n">
-        <v>1.896099391092399e-05</v>
-      </c>
-      <c r="KV12" t="n">
-        <v>5.450474782264791e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="KV12" t="inlineStr"/>
       <c r="KW12" t="n">
-        <v>0.4621845483779907</v>
+        <v>0.462</v>
       </c>
       <c r="KX12" t="n">
-        <v>2.51912522568668e-05</v>
+        <v>0</v>
       </c>
       <c r="KY12" t="inlineStr"/>
       <c r="KZ12" t="inlineStr"/>
       <c r="LA12" t="inlineStr"/>
-      <c r="LB12" t="n">
-        <v>5.540781421586871e-05</v>
-      </c>
+      <c r="LB12" t="inlineStr"/>
       <c r="LC12" t="n">
-        <v>0.4709209501743317</v>
+        <v>0.471</v>
       </c>
       <c r="LD12" t="n">
-        <v>2.609270051761974e-05</v>
+        <v>0</v>
       </c>
       <c r="LE12" t="inlineStr"/>
       <c r="LF12" t="inlineStr"/>
@@ -7739,23 +7473,19 @@
       <c r="LH12" t="inlineStr"/>
       <c r="LI12" t="inlineStr"/>
       <c r="LJ12" t="inlineStr"/>
-      <c r="LK12" t="n">
-        <v>5.147504271008074e-05</v>
-      </c>
+      <c r="LK12" t="inlineStr"/>
       <c r="LL12" t="n">
-        <v>0.5934224724769592</v>
+        <v>0.593</v>
       </c>
       <c r="LM12" t="n">
-        <v>3.054644711587319e-05</v>
-      </c>
-      <c r="LN12" t="n">
-        <v>6.163049692986533e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="LN12" t="inlineStr"/>
       <c r="LO12" t="n">
-        <v>0.4800974130630493</v>
+        <v>0.48</v>
       </c>
       <c r="LP12" t="n">
-        <v>2.958864214181855e-05</v>
+        <v>0</v>
       </c>
       <c r="LQ12" t="inlineStr"/>
       <c r="LR12" t="inlineStr"/>
@@ -7786,13 +7516,13 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="n">
-        <v>0.7303696274757385</v>
+        <v>0.73</v>
       </c>
       <c r="U13" t="n">
-        <v>0.3129585087299347</v>
+        <v>0.313</v>
       </c>
       <c r="V13" t="n">
-        <v>0.2285753894364451</v>
+        <v>0.229</v>
       </c>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
@@ -7804,13 +7534,13 @@
       <c r="AD13" t="inlineStr"/>
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="n">
-        <v>0.9494352340698242</v>
+        <v>0.949</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.3330029845237732</v>
+        <v>0.333</v>
       </c>
       <c r="AH13" t="n">
-        <v>0.3161647665572787</v>
+        <v>0.316</v>
       </c>
       <c r="AI13" t="inlineStr"/>
       <c r="AJ13" t="inlineStr"/>
@@ -7819,133 +7549,125 @@
       <c r="AM13" t="inlineStr"/>
       <c r="AN13" t="inlineStr"/>
       <c r="AO13" t="n">
-        <v>0.8708350658416748</v>
+        <v>0.871</v>
       </c>
       <c r="AP13" t="n">
-        <v>0.293449878692627</v>
+        <v>0.293</v>
       </c>
       <c r="AQ13" t="n">
-        <v>0.2555464444325253</v>
+        <v>0.256</v>
       </c>
       <c r="AR13" t="n">
-        <v>0.9210032224655151</v>
+        <v>0.921</v>
       </c>
       <c r="AS13" t="n">
-        <v>0.3430134654045105</v>
+        <v>0.343</v>
       </c>
       <c r="AT13" t="n">
-        <v>0.3159165069866177</v>
-      </c>
-      <c r="AU13" t="n">
-        <v>0.0003668662684503943</v>
-      </c>
+        <v>0.316</v>
+      </c>
+      <c r="AU13" t="inlineStr"/>
       <c r="AV13" t="n">
-        <v>0.3094916939735413</v>
+        <v>0.309</v>
       </c>
       <c r="AW13" t="n">
-        <v>0.0001135420628844645</v>
+        <v>0</v>
       </c>
       <c r="AX13" t="n">
-        <v>0.003599971532821655</v>
+        <v>0.004</v>
       </c>
       <c r="AY13" t="n">
-        <v>0.335444301366806</v>
+        <v>0.335</v>
       </c>
       <c r="AZ13" t="n">
-        <v>0.00120758993576775</v>
+        <v>0.001</v>
       </c>
       <c r="BA13" t="n">
-        <v>0.001273826928809285</v>
+        <v>0.001</v>
       </c>
       <c r="BB13" t="n">
-        <v>0.3283112347126007</v>
+        <v>0.328</v>
       </c>
       <c r="BC13" t="n">
-        <v>0.0004182116918075365</v>
+        <v>0</v>
       </c>
       <c r="BD13" t="inlineStr"/>
       <c r="BE13" t="inlineStr"/>
       <c r="BF13" t="inlineStr"/>
       <c r="BG13" t="n">
-        <v>0.8186301589012146</v>
+        <v>0.819</v>
       </c>
       <c r="BH13" t="n">
-        <v>0.3421033620834351</v>
+        <v>0.342</v>
       </c>
       <c r="BI13" t="n">
-        <v>0.2800561296630022</v>
-      </c>
-      <c r="BJ13" t="n">
-        <v>0.0003230697475373745</v>
-      </c>
+        <v>0.28</v>
+      </c>
+      <c r="BJ13" t="inlineStr"/>
       <c r="BK13" t="n">
-        <v>0.3044034242630005</v>
+        <v>0.304</v>
       </c>
       <c r="BL13" t="n">
-        <v>9.834353742615987e-05</v>
-      </c>
-      <c r="BM13" t="n">
-        <v>0.0003212481387890875</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="BM13" t="inlineStr"/>
       <c r="BN13" t="n">
-        <v>0.3017316460609436</v>
+        <v>0.302</v>
       </c>
       <c r="BO13" t="n">
-        <v>9.693072971084585e-05</v>
+        <v>0</v>
       </c>
       <c r="BP13" t="n">
-        <v>0.0008769098785705864</v>
+        <v>0.001</v>
       </c>
       <c r="BQ13" t="n">
-        <v>0.3303597867488861</v>
+        <v>0.33</v>
       </c>
       <c r="BR13" t="n">
-        <v>0.0002896957604825705</v>
+        <v>0</v>
       </c>
       <c r="BS13" t="n">
-        <v>0.04304348677396774</v>
+        <v>0.043</v>
       </c>
       <c r="BT13" t="n">
-        <v>0.323220282793045</v>
+        <v>0.323</v>
       </c>
       <c r="BU13" t="n">
-        <v>0.01391252796748055</v>
-      </c>
-      <c r="BV13" t="n">
-        <v>0.0004587786388583481</v>
-      </c>
+        <v>0.014</v>
+      </c>
+      <c r="BV13" t="inlineStr"/>
       <c r="BW13" t="n">
-        <v>0.3384907841682434</v>
+        <v>0.338</v>
       </c>
       <c r="BX13" t="n">
-        <v>0.0001552923412268016</v>
+        <v>0</v>
       </c>
       <c r="BY13" t="n">
-        <v>0.8803907036781311</v>
+        <v>0.88</v>
       </c>
       <c r="BZ13" t="n">
-        <v>0.3082703053951263</v>
+        <v>0.308</v>
       </c>
       <c r="CA13" t="n">
-        <v>0.2713983110898877</v>
+        <v>0.271</v>
       </c>
       <c r="CB13" t="n">
-        <v>0.9155679941177368</v>
+        <v>0.916</v>
       </c>
       <c r="CC13" t="n">
-        <v>0.3269670009613037</v>
+        <v>0.327</v>
       </c>
       <c r="CD13" t="n">
-        <v>0.299360521212833</v>
+        <v>0.299</v>
       </c>
       <c r="CE13" t="n">
-        <v>0.00266885501332581</v>
+        <v>0.003</v>
       </c>
       <c r="CF13" t="n">
-        <v>0.3167093694210052</v>
+        <v>0.317</v>
       </c>
       <c r="CG13" t="n">
-        <v>0.000845251388346506</v>
+        <v>0.001</v>
       </c>
       <c r="CH13" t="inlineStr"/>
       <c r="CI13" t="inlineStr"/>
@@ -7953,23 +7675,19 @@
       <c r="CK13" t="inlineStr"/>
       <c r="CL13" t="inlineStr"/>
       <c r="CM13" t="inlineStr"/>
-      <c r="CN13" t="n">
-        <v>0.0003061268944293261</v>
-      </c>
+      <c r="CN13" t="inlineStr"/>
       <c r="CO13" t="n">
-        <v>0.2991305589675903</v>
+        <v>0.299</v>
       </c>
       <c r="CP13" t="n">
-        <v>9.157190904565682e-05</v>
-      </c>
-      <c r="CQ13" t="n">
-        <v>0.0003066874924115837</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="CQ13" t="inlineStr"/>
       <c r="CR13" t="n">
-        <v>0.2965526580810547</v>
+        <v>0.297</v>
       </c>
       <c r="CS13" t="n">
-        <v>9.094899107486842e-05</v>
+        <v>0</v>
       </c>
       <c r="CT13" t="inlineStr"/>
       <c r="CU13" t="inlineStr"/>
@@ -7989,14 +7707,12 @@
       <c r="DI13" t="inlineStr"/>
       <c r="DJ13" t="inlineStr"/>
       <c r="DK13" t="inlineStr"/>
-      <c r="DL13" t="n">
-        <v>0.0003019278519786894</v>
-      </c>
+      <c r="DL13" t="inlineStr"/>
       <c r="DM13" t="n">
-        <v>0.3320285677909851</v>
+        <v>0.332</v>
       </c>
       <c r="DN13" t="n">
-        <v>0.0001002486722686928</v>
+        <v>0</v>
       </c>
       <c r="DO13" t="inlineStr"/>
       <c r="DP13" t="inlineStr"/>
@@ -8014,25 +7730,25 @@
       <c r="EB13" t="inlineStr"/>
       <c r="EC13" t="inlineStr"/>
       <c r="ED13" t="n">
-        <v>0.0005353499436751008</v>
+        <v>0.001</v>
       </c>
       <c r="EE13" t="n">
-        <v>0.3354441523551941</v>
+        <v>0.335</v>
       </c>
       <c r="EF13" t="n">
-        <v>0.0001795800080694951</v>
+        <v>0</v>
       </c>
       <c r="EG13" t="inlineStr"/>
       <c r="EH13" t="inlineStr"/>
       <c r="EI13" t="inlineStr"/>
       <c r="EJ13" t="n">
-        <v>0.009684748947620392</v>
+        <v>0.01</v>
       </c>
       <c r="EK13" t="n">
-        <v>0.3295685350894928</v>
+        <v>0.33</v>
       </c>
       <c r="EL13" t="n">
-        <v>0.00319178852337676</v>
+        <v>0.003</v>
       </c>
       <c r="EM13" t="inlineStr"/>
       <c r="EN13" t="inlineStr"/>
@@ -8047,13 +7763,13 @@
       <c r="EW13" t="inlineStr"/>
       <c r="EX13" t="inlineStr"/>
       <c r="EY13" t="n">
-        <v>0.004758525174111128</v>
+        <v>0.005</v>
       </c>
       <c r="EZ13" t="n">
-        <v>0.3326597511768341</v>
+        <v>0.333</v>
       </c>
       <c r="FA13" t="n">
-        <v>0.001582969800388509</v>
+        <v>0.002</v>
       </c>
       <c r="FB13" t="inlineStr"/>
       <c r="FC13" t="inlineStr"/>
@@ -8065,13 +7781,13 @@
       <c r="FI13" t="inlineStr"/>
       <c r="FJ13" t="inlineStr"/>
       <c r="FK13" t="n">
-        <v>0.0006760052056051791</v>
+        <v>0.001</v>
       </c>
       <c r="FL13" t="n">
-        <v>0.3230756223201752</v>
+        <v>0.323</v>
       </c>
       <c r="FM13" t="n">
-        <v>0.0002184008024925712</v>
+        <v>0</v>
       </c>
       <c r="FN13" t="inlineStr"/>
       <c r="FO13" t="inlineStr"/>
@@ -8079,14 +7795,12 @@
       <c r="FQ13" t="inlineStr"/>
       <c r="FR13" t="inlineStr"/>
       <c r="FS13" t="inlineStr"/>
-      <c r="FT13" t="n">
-        <v>0.00049714429769665</v>
-      </c>
+      <c r="FT13" t="inlineStr"/>
       <c r="FU13" t="n">
-        <v>0.2869135737419128</v>
+        <v>0.287</v>
       </c>
       <c r="FV13" t="n">
-        <v>0.0001426374471175593</v>
+        <v>0</v>
       </c>
       <c r="FW13" t="inlineStr"/>
       <c r="FX13" t="inlineStr"/>
@@ -8094,23 +7808,19 @@
       <c r="FZ13" t="inlineStr"/>
       <c r="GA13" t="inlineStr"/>
       <c r="GB13" t="inlineStr"/>
-      <c r="GC13" t="n">
-        <v>0.0002705521474126726</v>
-      </c>
+      <c r="GC13" t="inlineStr"/>
       <c r="GD13" t="n">
-        <v>0.3392732441425323</v>
+        <v>0.339</v>
       </c>
       <c r="GE13" t="n">
-        <v>9.179110476242609e-05</v>
-      </c>
-      <c r="GF13" t="n">
-        <v>0.0002629999944474548</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="GF13" t="inlineStr"/>
       <c r="GG13" t="n">
-        <v>0.316808819770813</v>
+        <v>0.317</v>
       </c>
       <c r="GH13" t="n">
-        <v>8.332071784062853e-05</v>
+        <v>0</v>
       </c>
       <c r="GI13" t="inlineStr"/>
       <c r="GJ13" t="inlineStr"/>
@@ -8121,23 +7831,21 @@
       <c r="GO13" t="inlineStr"/>
       <c r="GP13" t="inlineStr"/>
       <c r="GQ13" t="inlineStr"/>
-      <c r="GR13" t="n">
-        <v>0.0002944791631307453</v>
-      </c>
+      <c r="GR13" t="inlineStr"/>
       <c r="GS13" t="n">
-        <v>0.3165445923805237</v>
+        <v>0.317</v>
       </c>
       <c r="GT13" t="n">
-        <v>9.321578665777951e-05</v>
+        <v>0</v>
       </c>
       <c r="GU13" t="n">
-        <v>0.0006426931358873844</v>
+        <v>0.001</v>
       </c>
       <c r="GV13" t="n">
-        <v>0.3433759212493896</v>
+        <v>0.343</v>
       </c>
       <c r="GW13" t="n">
-        <v>0.0002206853476159898</v>
+        <v>0</v>
       </c>
       <c r="GX13" t="inlineStr"/>
       <c r="GY13" t="inlineStr"/>
@@ -8151,26 +7859,24 @@
       <c r="HG13" t="inlineStr"/>
       <c r="HH13" t="inlineStr"/>
       <c r="HI13" t="inlineStr"/>
-      <c r="HJ13" t="n">
-        <v>0.0002728878462221473</v>
-      </c>
+      <c r="HJ13" t="inlineStr"/>
       <c r="HK13" t="n">
-        <v>0.331915020942688</v>
+        <v>0.332</v>
       </c>
       <c r="HL13" t="n">
-        <v>9.057557519382906e-05</v>
+        <v>0</v>
       </c>
       <c r="HM13" t="inlineStr"/>
       <c r="HN13" t="inlineStr"/>
       <c r="HO13" t="inlineStr"/>
       <c r="HP13" t="n">
-        <v>0.002330499235540628</v>
+        <v>0.002</v>
       </c>
       <c r="HQ13" t="n">
-        <v>0.3283557891845703</v>
+        <v>0.328</v>
       </c>
       <c r="HR13" t="n">
-        <v>0.0007652329156799809</v>
+        <v>0.001</v>
       </c>
       <c r="HS13" t="inlineStr"/>
       <c r="HT13" t="inlineStr"/>
@@ -8211,26 +7917,24 @@
       <c r="JC13" t="inlineStr"/>
       <c r="JD13" t="inlineStr"/>
       <c r="JE13" t="inlineStr"/>
-      <c r="JF13" t="n">
-        <v>0.0004286401090212166</v>
-      </c>
+      <c r="JF13" t="inlineStr"/>
       <c r="JG13" t="n">
-        <v>0.3121208846569061</v>
+        <v>0.312</v>
       </c>
       <c r="JH13" t="n">
-        <v>0.0001337875300271348</v>
+        <v>0</v>
       </c>
       <c r="JI13" t="inlineStr"/>
       <c r="JJ13" t="inlineStr"/>
       <c r="JK13" t="inlineStr"/>
       <c r="JL13" t="n">
-        <v>0.001842074445448816</v>
+        <v>0.002</v>
       </c>
       <c r="JM13" t="n">
-        <v>0.3198650479316711</v>
+        <v>0.32</v>
       </c>
       <c r="JN13" t="n">
-        <v>0.000589215230787192</v>
+        <v>0.001</v>
       </c>
       <c r="JO13" t="inlineStr"/>
       <c r="JP13" t="inlineStr"/>
@@ -8251,13 +7955,13 @@
       <c r="KE13" t="inlineStr"/>
       <c r="KF13" t="inlineStr"/>
       <c r="KG13" t="n">
-        <v>0.0008973876829259098</v>
+        <v>0.001</v>
       </c>
       <c r="KH13" t="n">
-        <v>0.3178973793983459</v>
+        <v>0.318</v>
       </c>
       <c r="KI13" t="n">
-        <v>0.0002852771927065005</v>
+        <v>0</v>
       </c>
       <c r="KJ13" t="inlineStr"/>
       <c r="KK13" t="inlineStr"/>
@@ -8275,13 +7979,13 @@
       <c r="KW13" t="inlineStr"/>
       <c r="KX13" t="inlineStr"/>
       <c r="KY13" t="n">
-        <v>0.2594442963600159</v>
+        <v>0.259</v>
       </c>
       <c r="KZ13" t="n">
-        <v>0.3078318536281586</v>
+        <v>0.308</v>
       </c>
       <c r="LA13" t="n">
-        <v>0.079865218661757</v>
+        <v>0.08</v>
       </c>
       <c r="LB13" t="inlineStr"/>
       <c r="LC13" t="inlineStr"/>
@@ -8324,25 +8028,25 @@
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="n">
-        <v>0.03536398336291313</v>
+        <v>0.035</v>
       </c>
       <c r="R14" t="n">
-        <v>0.1693228334188461</v>
+        <v>0.169</v>
       </c>
       <c r="S14" t="n">
-        <v>0.005987929863985386</v>
+        <v>0.006</v>
       </c>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
       <c r="W14" t="n">
-        <v>0.05155674368143082</v>
+        <v>0.052</v>
       </c>
       <c r="X14" t="n">
-        <v>0.2439930588006973</v>
+        <v>0.244</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.01257948759263583</v>
+        <v>0.013</v>
       </c>
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="inlineStr"/>
@@ -8375,13 +8079,13 @@
       <c r="BB14" t="inlineStr"/>
       <c r="BC14" t="inlineStr"/>
       <c r="BD14" t="n">
-        <v>0.1038120239973068</v>
+        <v>0.104</v>
       </c>
       <c r="BE14" t="n">
-        <v>0.2716616094112396</v>
+        <v>0.272</v>
       </c>
       <c r="BF14" t="n">
-        <v>0.0282017415153466</v>
+        <v>0.028</v>
       </c>
       <c r="BG14" t="inlineStr"/>
       <c r="BH14" t="inlineStr"/>
@@ -8423,13 +8127,13 @@
       <c r="CR14" t="inlineStr"/>
       <c r="CS14" t="inlineStr"/>
       <c r="CT14" t="n">
-        <v>0.06854385137557983</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="CU14" t="n">
-        <v>0.2119921892881393</v>
+        <v>0.212</v>
       </c>
       <c r="CV14" t="n">
-        <v>0.01453076111535001</v>
+        <v>0.015</v>
       </c>
       <c r="CW14" t="inlineStr"/>
       <c r="CX14" t="inlineStr"/>
@@ -8444,13 +8148,13 @@
       <c r="DG14" t="inlineStr"/>
       <c r="DH14" t="inlineStr"/>
       <c r="DI14" t="n">
-        <v>0.1162607297301292</v>
+        <v>0.116</v>
       </c>
       <c r="DJ14" t="n">
-        <v>0.1961047500371933</v>
+        <v>0.196</v>
       </c>
       <c r="DK14" t="n">
-        <v>0.02279928134286868</v>
+        <v>0.023</v>
       </c>
       <c r="DL14" t="inlineStr"/>
       <c r="DM14" t="inlineStr"/>
@@ -8474,13 +8178,13 @@
       <c r="EE14" t="inlineStr"/>
       <c r="EF14" t="inlineStr"/>
       <c r="EG14" t="n">
-        <v>0.1412228345870972</v>
+        <v>0.141</v>
       </c>
       <c r="EH14" t="n">
-        <v>0.194097176194191</v>
+        <v>0.194</v>
       </c>
       <c r="EI14" t="n">
-        <v>0.02741095340749489</v>
+        <v>0.027</v>
       </c>
       <c r="EJ14" t="inlineStr"/>
       <c r="EK14" t="inlineStr"/>
@@ -8495,25 +8199,25 @@
       <c r="ET14" t="inlineStr"/>
       <c r="EU14" t="inlineStr"/>
       <c r="EV14" t="n">
-        <v>0.1810628771781921</v>
+        <v>0.181</v>
       </c>
       <c r="EW14" t="n">
-        <v>0.1783688217401505</v>
+        <v>0.178</v>
       </c>
       <c r="EX14" t="n">
-        <v>0.03229597206315571</v>
+        <v>0.032</v>
       </c>
       <c r="EY14" t="inlineStr"/>
       <c r="EZ14" t="inlineStr"/>
       <c r="FA14" t="inlineStr"/>
       <c r="FB14" t="n">
-        <v>0.2089017331600189</v>
+        <v>0.209</v>
       </c>
       <c r="FC14" t="n">
-        <v>0.1564267575740814</v>
+        <v>0.156</v>
       </c>
       <c r="FD14" t="n">
-        <v>0.03267782076982773</v>
+        <v>0.033</v>
       </c>
       <c r="FE14" t="inlineStr"/>
       <c r="FF14" t="inlineStr"/>
@@ -8537,13 +8241,13 @@
       <c r="FX14" t="inlineStr"/>
       <c r="FY14" t="inlineStr"/>
       <c r="FZ14" t="n">
-        <v>0.1338474601507187</v>
+        <v>0.134</v>
       </c>
       <c r="GA14" t="n">
-        <v>0.1756714880466461</v>
+        <v>0.176</v>
       </c>
       <c r="GB14" t="n">
-        <v>0.02351318249594092</v>
+        <v>0.024</v>
       </c>
       <c r="GC14" t="inlineStr"/>
       <c r="GD14" t="inlineStr"/>
@@ -8591,22 +8295,22 @@
       <c r="HT14" t="inlineStr"/>
       <c r="HU14" t="inlineStr"/>
       <c r="HV14" t="n">
-        <v>0.1063855811953545</v>
+        <v>0.106</v>
       </c>
       <c r="HW14" t="n">
-        <v>0.1812639236450195</v>
+        <v>0.181</v>
       </c>
       <c r="HX14" t="n">
-        <v>0.01928386786672576</v>
+        <v>0.019</v>
       </c>
       <c r="HY14" t="n">
-        <v>0.1795501112937927</v>
+        <v>0.18</v>
       </c>
       <c r="HZ14" t="n">
-        <v>0.1967543214559555</v>
+        <v>0.197</v>
       </c>
       <c r="IA14" t="n">
-        <v>0.03532726031495148</v>
+        <v>0.035</v>
       </c>
       <c r="IB14" t="inlineStr"/>
       <c r="IC14" t="inlineStr"/>
@@ -8624,34 +8328,34 @@
       <c r="IO14" t="inlineStr"/>
       <c r="IP14" t="inlineStr"/>
       <c r="IQ14" t="n">
-        <v>0.1637964844703674</v>
+        <v>0.164</v>
       </c>
       <c r="IR14" t="n">
-        <v>0.2046879827976227</v>
+        <v>0.205</v>
       </c>
       <c r="IS14" t="n">
-        <v>0.03352717199558164</v>
+        <v>0.034</v>
       </c>
       <c r="IT14" t="n">
-        <v>0.1774988174438477</v>
+        <v>0.177</v>
       </c>
       <c r="IU14" t="n">
-        <v>0.2112432867288589</v>
+        <v>0.211</v>
       </c>
       <c r="IV14" t="n">
-        <v>0.0374954335873241</v>
+        <v>0.037</v>
       </c>
       <c r="IW14" t="inlineStr"/>
       <c r="IX14" t="inlineStr"/>
       <c r="IY14" t="inlineStr"/>
       <c r="IZ14" t="n">
-        <v>0.167897030711174</v>
+        <v>0.168</v>
       </c>
       <c r="JA14" t="n">
-        <v>0.2128784209489822</v>
+        <v>0.213</v>
       </c>
       <c r="JB14" t="n">
-        <v>0.0357416547798175</v>
+        <v>0.036</v>
       </c>
       <c r="JC14" t="inlineStr"/>
       <c r="JD14" t="inlineStr"/>
@@ -8681,13 +8385,13 @@
       <c r="KB14" t="inlineStr"/>
       <c r="KC14" t="inlineStr"/>
       <c r="KD14" t="n">
-        <v>0.342393547296524</v>
+        <v>0.342</v>
       </c>
       <c r="KE14" t="n">
-        <v>0.1971946358680725</v>
+        <v>0.197</v>
       </c>
       <c r="KF14" t="n">
-        <v>0.06751817088271572</v>
+        <v>0.068</v>
       </c>
       <c r="KG14" t="inlineStr"/>
       <c r="KH14" t="inlineStr"/>
@@ -8714,13 +8418,13 @@
       <c r="LC14" t="inlineStr"/>
       <c r="LD14" t="inlineStr"/>
       <c r="LE14" t="n">
-        <v>0.1768949925899506</v>
+        <v>0.177</v>
       </c>
       <c r="LF14" t="n">
-        <v>0.1797441989183426</v>
+        <v>0.18</v>
       </c>
       <c r="LG14" t="n">
-        <v>0.03179584873574681</v>
+        <v>0.032</v>
       </c>
       <c r="LH14" t="inlineStr"/>
       <c r="LI14" t="inlineStr"/>
@@ -8732,13 +8436,13 @@
       <c r="LO14" t="inlineStr"/>
       <c r="LP14" t="inlineStr"/>
       <c r="LQ14" t="n">
-        <v>0.1455947607755661</v>
+        <v>0.146</v>
       </c>
       <c r="LR14" t="n">
-        <v>0.2056462615728378</v>
+        <v>0.206</v>
       </c>
       <c r="LS14" t="n">
-        <v>0.02994101825808682</v>
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>